<commit_message>
SRS and Github Review is covered
</commit_message>
<xml_diff>
--- a/Monitor and Control/F_Review.xlsx
+++ b/Monitor and Control/F_Review.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9652312A-C8D1-43DD-90CF-BBA140D3012C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="12456" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP_Review" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Audit_Review!$A$1:$L$1</definedName>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="213">
   <si>
     <t>Raised By</t>
   </si>
@@ -688,11 +687,35 @@
   <si>
     <t>WireFrame_Review</t>
   </si>
+  <si>
+    <t>F_REVIEW_Audit_V1.0_021</t>
+  </si>
+  <si>
+    <t>only one version of SRS</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Audit_V1.0_022</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Audit_V1.0_023</t>
+  </si>
+  <si>
+    <t>empty revision history</t>
+  </si>
+  <si>
+    <t>only old document is uploaded</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Audit_V1.0_024</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Audit_V1.0_025</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
@@ -941,7 +964,63 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="168">
+  <dxfs count="176">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2176,7 +2255,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2288,7 +2366,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -2312,7 +2389,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2323,7 +2399,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -2347,7 +2422,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2358,7 +2432,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -2382,7 +2455,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2393,7 +2465,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -2456,7 +2527,6 @@
                       <a:avLst/>
                     </a:prstGeom>
                   </c15:spPr>
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2589,7 +2659,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2671,7 +2740,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2803,7 +2871,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -2866,7 +2933,6 @@
                       <a:avLst/>
                     </a:prstGeom>
                   </c15:spPr>
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2877,7 +2943,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -2901,7 +2966,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2912,7 +2976,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -2936,7 +2999,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2947,7 +3009,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -2971,7 +3032,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3104,7 +3164,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3216,7 +3275,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3343,7 +3401,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -3367,7 +3424,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3378,7 +3434,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -3402,7 +3457,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3413,7 +3467,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -3437,7 +3490,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3448,7 +3500,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -3472,7 +3523,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3605,7 +3655,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3687,7 +3736,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3814,7 +3862,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -3838,7 +3885,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3849,7 +3895,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -3873,7 +3918,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3884,7 +3928,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -3908,7 +3951,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3919,7 +3961,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -3943,7 +3984,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4076,7 +4116,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4158,7 +4197,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4285,7 +4323,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -4309,7 +4346,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4320,7 +4356,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -4344,7 +4379,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4355,7 +4389,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -4379,7 +4412,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4390,7 +4422,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -4414,7 +4445,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4546,7 +4576,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4628,7 +4657,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4755,7 +4783,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -4779,7 +4806,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4790,7 +4816,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -4814,7 +4839,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4825,7 +4849,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -4849,7 +4872,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4860,7 +4882,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -4884,7 +4905,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4978,7 +4998,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -5016,7 +5036,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7802,7 +7821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8283,44 +8302,44 @@
     <mergeCell ref="B16:J16"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F15 F18:F1048576">
-    <cfRule type="cellIs" dxfId="167" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="10" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="163" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="6" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="159" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8329,7 +8348,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Options!$B$1:$B$4</xm:f>
           </x14:formula1>
@@ -8342,7 +8361,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8380,7 +8399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8610,16 +8629,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="155" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8628,7 +8647,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>Options!$B$1:$B$4</xm:f>
           </x14:formula1>
@@ -8641,7 +8660,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView topLeftCell="B1048548" workbookViewId="0">
@@ -9040,156 +9059,156 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F14:F21 F23:F1048576 F1:F3">
-    <cfRule type="cellIs" dxfId="151" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="41" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="42" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="43" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="44" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="147" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="37" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="38" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="39" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="40" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="143" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="33" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="34" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="35" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="36" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="139" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="29" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="30" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="31" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="32" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="135" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="25" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="26" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="27" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="28" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="131" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="21" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="22" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="23" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="127" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="17" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="18" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="19" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="123" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="14" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="15" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="119" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="115" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="111" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9198,7 +9217,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>Options!$B$1:$B$4</xm:f>
           </x14:formula1>
@@ -9211,7 +9230,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9829,16 +9848,16 @@
     <mergeCell ref="B13:J13"/>
   </mergeCells>
   <conditionalFormatting sqref="F14:F21 F23:F1048576 F1:F12">
-    <cfRule type="cellIs" dxfId="107" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9847,7 +9866,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>Options!$B$1:$B$4</xm:f>
           </x14:formula1>
@@ -9860,7 +9879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10032,16 +10051,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F14:F21 F23:F1048576 F1:F12">
-    <cfRule type="cellIs" dxfId="103" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10049,7 +10068,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
             <xm:f>Options!$B$1:$B$4</xm:f>
           </x14:formula1>
@@ -10062,14 +10081,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10:L10"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10809,54 +10828,364 @@
         <v>107</v>
       </c>
     </row>
+    <row r="23" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="10">
+        <v>44686</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J23" s="10">
+        <v>44686</v>
+      </c>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="10">
+        <v>44686</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J24" s="10">
+        <v>44686</v>
+      </c>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="10">
+        <v>44686</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J25" s="10">
+        <v>44686</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="10">
+        <v>44686</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J26" s="10">
+        <v>44686</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="10">
+        <v>44686</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J27" s="10">
+        <v>44686</v>
+      </c>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L1"/>
+  <autoFilter ref="A1:L1" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A10:L10"/>
   </mergeCells>
-  <conditionalFormatting sqref="H23:H1048576">
-    <cfRule type="cellIs" dxfId="95" priority="129" operator="equal">
+  <conditionalFormatting sqref="H28:H1048576">
+    <cfRule type="cellIs" dxfId="107" priority="185" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="186" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="187" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="188" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="101" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="102" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="103" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="104" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="97" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="98" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="99" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="100" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H16">
+    <cfRule type="cellIs" dxfId="95" priority="93" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="94" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="95" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="96" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H16">
+    <cfRule type="cellIs" dxfId="91" priority="89" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="90" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="91" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="92" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="cellIs" dxfId="87" priority="77" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="78" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="79" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="80" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="cellIs" dxfId="83" priority="73" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="74" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="75" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="76" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17:H20">
+    <cfRule type="cellIs" dxfId="79" priority="85" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="86" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="87" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="88" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17:H20">
+    <cfRule type="cellIs" dxfId="75" priority="81" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="82" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="83" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="84" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="cellIs" dxfId="71" priority="69" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="70" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="71" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="cellIs" dxfId="67" priority="65" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="68" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H9">
+    <cfRule type="cellIs" dxfId="63" priority="61" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="62" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="63" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="64" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H9">
+    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="59" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
     <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -10870,7 +11199,7 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H16">
+  <conditionalFormatting sqref="H23">
     <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -10884,63 +11213,63 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+  <conditionalFormatting sqref="H25">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
+  <conditionalFormatting sqref="H25">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
+  <conditionalFormatting sqref="H26">
     <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -10954,7 +11283,7 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
+  <conditionalFormatting sqref="H26">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -10968,7 +11297,7 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H9">
+  <conditionalFormatting sqref="H27">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -10982,7 +11311,7 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H27">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -11001,17 +11330,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000000000000}">
           <x14:formula1>
             <xm:f>Options!$B$1:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H23:H1048576</xm:sqref>
+          <xm:sqref>H28:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
           <x14:formula1>
-            <xm:f>[F_Review.xlsx]Options!#REF!</xm:f>
+            <xm:f>Options!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>H11:H22 H1:H9</xm:sqref>
+          <xm:sqref>H1:H9 H11:H27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11020,7 +11349,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A3:N46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -11263,7 +11592,7 @@
       </c>
       <c r="N43" s="24">
         <f>COUNTIF(Audit_Review!H2:H1048576,"Closed")</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
@@ -11317,7 +11646,7 @@
       </c>
       <c r="N46" s="24">
         <f>SUM(N42:N45)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
after eng mohamed aduit
</commit_message>
<xml_diff>
--- a/Monitor and Control/F_Review.xlsx
+++ b/Monitor and Control/F_Review.xlsx
@@ -3,26 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8004DDC3-89D0-4911-BDE5-94F78B126EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355859A6-D5CE-49E8-817D-9604C4FD6243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP_Review" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="5" state="hidden" r:id="rId2"/>
     <sheet name="Risk_Managment_Plan_Review" sheetId="7" r:id="rId3"/>
-    <sheet name="Scope_Statment_Review" sheetId="9" r:id="rId4"/>
-    <sheet name="WireFrame_Review" sheetId="12" r:id="rId5"/>
-    <sheet name="SRS_Review" sheetId="3" r:id="rId6"/>
-    <sheet name="Sequence_Diagrams_Review" sheetId="10" r:id="rId7"/>
-    <sheet name="Audit_Review" sheetId="11" r:id="rId8"/>
-    <sheet name="Progress_Chart" sheetId="4" r:id="rId9"/>
+    <sheet name="WireFrame_Review" sheetId="12" r:id="rId4"/>
+    <sheet name="SRS_Review" sheetId="3" r:id="rId5"/>
+    <sheet name="Sequence_Diagrams_Review" sheetId="10" r:id="rId6"/>
+    <sheet name="Audit_Review" sheetId="11" r:id="rId7"/>
+    <sheet name="Progress_Chart" sheetId="4" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Audit_Review!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Audit_Review!$A$1:$L$1</definedName>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -42,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="221">
   <si>
     <t>Raised By</t>
   </si>
@@ -178,9 +175,6 @@
     <t>Closed By</t>
   </si>
   <si>
-    <t>In page 1 in scope description in the in scope section this part " Search engine optimized nearby Restaurants" should be changed according to our update we got from the review</t>
-  </si>
-  <si>
     <t xml:space="preserve">section 3.22 has a conflict topic </t>
   </si>
   <si>
@@ -253,23 +247,7 @@
     <t>Need Approval</t>
   </si>
   <si>
-    <t>Assign To</t>
-  </si>
-  <si>
     <t>Aml Nasser</t>
-  </si>
-  <si>
-    <t>In page 1 the launching date must change to the fifth week 
-(is not determined yet)</t>
-  </si>
-  <si>
-    <t>Scope_Statement</t>
-  </si>
-  <si>
-    <t>F_REVIEW_SS_V1.0_001</t>
-  </si>
-  <si>
-    <t>F_REVIEW_SS_V1.0_002</t>
   </si>
   <si>
     <t>F_REVIEW_RMP_V1.0_001</t>
@@ -665,6 +643,15 @@
   </si>
   <si>
     <t>In the Home page, please change "Restraunt menu" title to "Foodies' Restraunts" as this is the page that contains the restraunts themselves not the restraunt menus.</t>
+  </si>
+  <si>
+    <t>in the nav bar a link to the home page must be added</t>
+  </si>
+  <si>
+    <t>what happen if the user forget his password</t>
+  </si>
+  <si>
+    <t>a link to the home and menu must be added</t>
   </si>
   <si>
     <r>
@@ -693,6 +680,60 @@
   </si>
   <si>
     <t>I changed the sequence due to look and feel concepts</t>
+  </si>
+  <si>
+    <t>Need to go deep in each branch</t>
+  </si>
+  <si>
+    <t>WireFrame_Review</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Audit_V1.0_021</t>
+  </si>
+  <si>
+    <t>only one version of SRS</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Audit_V1.0_022</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Audit_V1.0_023</t>
+  </si>
+  <si>
+    <t>empty revision history</t>
+  </si>
+  <si>
+    <t>only old document is uploaded</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Audit_V1.0_024</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Audit_V1.0_025</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Aduit_V1.3_0.26</t>
+  </si>
+  <si>
+    <t>ERD</t>
+  </si>
+  <si>
+    <t>USECASE</t>
+  </si>
+  <si>
+    <t>Update the version</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Aduit_V1.3_0.27</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Aduit_V1.3_0.28</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Aduit_V1.3_0.29</t>
+  </si>
+  <si>
+    <t>version consistency with the review sheet and version history</t>
   </si>
 </sst>
 </file>
@@ -757,7 +798,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -768,7 +809,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -828,12 +869,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -879,7 +940,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -904,6 +964,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -913,7 +979,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -943,7 +1020,259 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="124">
+  <dxfs count="160">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2737,10 +3066,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3228,10 +3557,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4610,16 +4939,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7443,7 +7772,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7455,19 +7784,19 @@
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="13.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="24.88671875" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>2</v>
@@ -7485,27 +7814,27 @@
         <v>5</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D2" s="10">
         <v>44664</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>6</v>
@@ -7521,13 +7850,13 @@
     </row>
     <row r="3" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D3" s="10">
         <v>44664</v>
@@ -7549,19 +7878,19 @@
     </row>
     <row r="4" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" s="10">
         <v>44664</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>6</v>
@@ -7577,13 +7906,13 @@
     </row>
     <row r="5" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" s="10">
         <v>44664</v>
@@ -7605,13 +7934,13 @@
     </row>
     <row r="6" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D6" s="10">
         <v>44664</v>
@@ -7633,13 +7962,13 @@
     </row>
     <row r="7" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D7" s="10">
         <v>44664</v>
@@ -7660,32 +7989,32 @@
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="34"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="10">
         <v>44678</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>6</v>
@@ -7701,19 +8030,19 @@
     </row>
     <row r="10" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" s="10">
         <v>44678</v>
       </c>
-      <c r="E10" s="20" t="s">
-        <v>90</v>
+      <c r="E10" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>6</v>
@@ -7729,19 +8058,19 @@
     </row>
     <row r="11" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D11" s="10">
         <v>44678</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>6</v>
@@ -7753,27 +8082,27 @@
         <v>44680</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" s="10">
         <v>44678</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>6</v>
@@ -7789,19 +8118,19 @@
     </row>
     <row r="13" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="10">
         <v>44678</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>6</v>
@@ -7817,19 +8146,19 @@
     </row>
     <row r="14" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="10">
         <v>44678</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>6</v>
@@ -7845,13 +8174,13 @@
     </row>
     <row r="15" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D15" s="10">
         <v>44678</v>
@@ -7860,40 +8189,44 @@
         <v>36</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="10">
+        <v>44680</v>
+      </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="34"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D17" s="10">
         <v>44680</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>6</v>
@@ -7913,44 +8246,44 @@
     <mergeCell ref="B16:J16"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F15 F18:F1048576">
-    <cfRule type="cellIs" dxfId="123" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="10" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="119" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="6" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="115" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7996,12 +8329,12 @@
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -8036,13 +8369,13 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>2</v>
@@ -8060,27 +8393,27 @@
         <v>5</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D2" s="10">
         <v>44678</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>6</v>
@@ -8096,13 +8429,13 @@
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D3" s="10">
         <v>44678</v>
@@ -8124,13 +8457,13 @@
     </row>
     <row r="4" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" s="10">
         <v>44678</v>
@@ -8152,13 +8485,13 @@
     </row>
     <row r="5" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" s="10">
         <v>44678</v>
@@ -8176,21 +8509,21 @@
         <v>44680</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D6" s="10">
         <v>44678</v>
@@ -8212,13 +8545,13 @@
     </row>
     <row r="7" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D7" s="10">
         <v>44678</v>
@@ -8240,16 +8573,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="111" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8272,167 +8605,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="24.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="79.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
-    <col min="9" max="10" width="24.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="10">
-        <v>44678</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="10">
-        <v>44680</v>
-      </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="10">
-        <v>44678</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="10">
-        <v>44680</v>
-      </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="F1:F2 F4:F1048576">
-    <cfRule type="cellIs" dxfId="107" priority="5" operator="equal">
-      <formula>"Need Approval"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="6" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="7" operator="equal">
-      <formula>"Closed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="8" operator="equal">
-      <formula>"Open"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="103" priority="1" operator="equal">
-      <formula>"Need Approval"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="2" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="3" operator="equal">
-      <formula>"Closed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="4" operator="equal">
-      <formula>"Open"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
-          <x14:formula1>
-            <xm:f>Options!$B$1:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8441,23 +8617,24 @@
     <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="16.109375" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="50.44140625" customWidth="1"/>
+    <col min="5" max="5" width="54" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" style="7" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="15.5546875" customWidth="1"/>
     <col min="9" max="9" width="34.6640625" customWidth="1"/>
     <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>2</v>
@@ -8475,34 +8652,32 @@
         <v>5</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D2" s="10">
         <v>44686</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>181</v>
-      </c>
+      <c r="G2" s="5"/>
       <c r="H2" s="10">
         <v>44687</v>
       </c>
@@ -8511,196 +8686,184 @@
     </row>
     <row r="3" spans="1:10" ht="122.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D3" s="10">
         <v>44686</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>181</v>
-      </c>
+      <c r="G3" s="5"/>
       <c r="H3" s="10">
         <v>44687</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" s="31" customFormat="1" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B4" s="28" t="s">
+    <row r="4" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="27">
+        <v>44686</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J4" s="28"/>
+    </row>
+    <row r="5" spans="1:10" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="D4" s="29">
+      <c r="B5" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="27">
         <v>44686</v>
       </c>
-      <c r="E4" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="F4" s="28" t="s">
+      <c r="E5" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="H4" s="29">
+      <c r="G5" s="26"/>
+      <c r="H5" s="27">
         <v>44687</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-    </row>
-    <row r="5" spans="1:10" s="31" customFormat="1" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="D5" s="29">
-        <v>44686</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="H5" s="29">
-        <v>44687</v>
-      </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
+      <c r="I5" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" spans="1:10" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D6" s="10">
         <v>44686</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>181</v>
-      </c>
+      <c r="G6" s="5"/>
       <c r="H6" s="10">
         <v>44687</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" s="31" customFormat="1" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="D7" s="29">
+    <row r="7" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="30">
         <v>44686</v>
       </c>
-      <c r="E7" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="F7" s="28" t="s">
+      <c r="E7" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="F7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="H7" s="29">
+      <c r="G7" s="29"/>
+      <c r="H7" s="30">
         <v>44687</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-    </row>
-    <row r="8" spans="1:10" s="31" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="D8" s="29">
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+    </row>
+    <row r="8" spans="1:10" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="27">
         <v>44686</v>
       </c>
-      <c r="E8" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="H8" s="29">
-        <v>44687</v>
-      </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
+      <c r="E8" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D9" s="10">
         <v>44686</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>181</v>
-      </c>
+      <c r="G9" s="5"/>
       <c r="H9" s="10">
         <v>44687</v>
       </c>
@@ -8709,26 +8872,24 @@
     </row>
     <row r="10" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D10" s="10">
         <v>44686</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>181</v>
-      </c>
+      <c r="G10" s="5"/>
       <c r="H10" s="10">
         <v>44687</v>
       </c>
@@ -8737,26 +8898,24 @@
     </row>
     <row r="11" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D11" s="10">
         <v>44686</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>181</v>
-      </c>
+      <c r="G11" s="5"/>
       <c r="H11" s="10">
         <v>44687</v>
       </c>
@@ -8765,26 +8924,24 @@
     </row>
     <row r="12" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D12" s="10">
         <v>44686</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>181</v>
-      </c>
+      <c r="G12" s="5"/>
       <c r="H12" s="10">
         <v>44687</v>
       </c>
@@ -8793,26 +8950,24 @@
     </row>
     <row r="13" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D13" s="10">
         <v>44686</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>181</v>
-      </c>
+      <c r="G13" s="5"/>
       <c r="H13" s="10">
         <v>44687</v>
       </c>
@@ -8820,184 +8975,184 @@
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F14" s="22"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F15" s="22"/>
+      <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F16" s="22"/>
+      <c r="F16" s="21"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F17" s="22"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F18" s="22"/>
+      <c r="F18" s="21"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F19" s="22"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F20" s="22"/>
+      <c r="F20" s="21"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F21" s="22"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F14:F21 F23:F1048576 F1:F3">
-    <cfRule type="cellIs" dxfId="99" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="41" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="42" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="43" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="44" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="95" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="37" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="38" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="39" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="40" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="91" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="33" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="34" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="35" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="36" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="87" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="29" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="30" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="31" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="32" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="83" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="25" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="26" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="27" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="28" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="79" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="21" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="22" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="23" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="75" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="17" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="18" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="19" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="71" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="14" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="15" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="67" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="63" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9006,7 +9161,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>Options!$B$1:$B$4</xm:f>
           </x14:formula1>
@@ -9018,8 +9173,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9045,13 +9200,13 @@
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>2</v>
@@ -9069,21 +9224,21 @@
         <v>5</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="10">
         <v>44664</v>
@@ -9100,18 +9255,18 @@
       <c r="H2" s="10">
         <v>44666</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="10">
         <v>44664</v>
@@ -9128,18 +9283,18 @@
       <c r="H3" s="10">
         <v>44666</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="10">
         <v>44664</v>
@@ -9156,18 +9311,18 @@
       <c r="H4" s="10">
         <v>44666</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="10">
         <v>44664</v>
@@ -9184,18 +9339,18 @@
       <c r="H5" s="10">
         <v>44666</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="10">
         <v>44664</v>
@@ -9212,18 +9367,18 @@
       <c r="H6" s="10">
         <v>44666</v>
       </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="10">
         <v>44664</v>
@@ -9240,24 +9395,24 @@
       <c r="H7" s="10">
         <v>44666</v>
       </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="10">
         <v>44664</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>6</v>
@@ -9268,18 +9423,18 @@
       <c r="H8" s="10">
         <v>44666</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="10">
         <v>44664</v>
@@ -9296,18 +9451,18 @@
       <c r="H9" s="10">
         <v>44666</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="10">
         <v>44664</v>
@@ -9324,18 +9479,18 @@
       <c r="H10" s="10">
         <v>44666</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="10">
         <v>44664</v>
@@ -9352,18 +9507,18 @@
       <c r="H11" s="10">
         <v>44666</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="10">
         <v>44664</v>
@@ -9380,30 +9535,30 @@
       <c r="H12" s="10">
         <v>44666</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="34"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="10">
         <v>44664</v>
@@ -9420,18 +9575,18 @@
       <c r="H14" s="10">
         <v>44666</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="10">
         <v>44664</v>
@@ -9448,18 +9603,18 @@
       <c r="H15" s="10">
         <v>44666</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="10">
         <v>44665</v>
@@ -9476,18 +9631,18 @@
       <c r="H16" s="10">
         <v>44666</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
     </row>
     <row r="17" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="10">
         <v>44666</v>
@@ -9504,18 +9659,18 @@
       <c r="H17" s="10">
         <v>44666</v>
       </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
     </row>
     <row r="18" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="10">
         <v>44666</v>
@@ -9532,18 +9687,18 @@
       <c r="H18" s="10">
         <v>44666</v>
       </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="10">
         <v>44666</v>
@@ -9560,18 +9715,18 @@
       <c r="H19" s="10">
         <v>44666</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
     </row>
     <row r="20" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="10">
         <v>44666</v>
@@ -9588,18 +9743,18 @@
       <c r="H20" s="10">
         <v>44666</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
     </row>
     <row r="21" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="10">
         <v>44666</v>
@@ -9616,20 +9771,20 @@
       <c r="H21" s="10">
         <v>44666</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="34"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9637,16 +9792,16 @@
     <mergeCell ref="B13:J13"/>
   </mergeCells>
   <conditionalFormatting sqref="F14:F21 F23:F1048576 F1:F12">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9655,7 +9810,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>Options!$B$1:$B$4</xm:f>
           </x14:formula1>
@@ -9667,12 +9822,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="A1:XFD1048576"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9691,13 +9846,13 @@
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>2</v>
@@ -9715,141 +9870,141 @@
         <v>5</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D2" s="10">
         <v>44680</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H2" s="10">
         <v>44680</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D3" s="10">
         <v>44680</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H3" s="10">
         <v>44680</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F4" s="22"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F5" s="22"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F6" s="22"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F7" s="22"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F8" s="22"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F9" s="22"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F10" s="22"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F11" s="22"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F12" s="22"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F13" s="23"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F14" s="22"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F15" s="22"/>
+      <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F16" s="22"/>
+      <c r="F16" s="21"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F17" s="22"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F18" s="22"/>
+      <c r="F18" s="21"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F19" s="22"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F20" s="22"/>
+      <c r="F20" s="21"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F21" s="22"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F14:F21 F23:F1048576 F1:F12">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9857,7 +10012,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
             <xm:f>Options!$B$1:$B$4</xm:f>
           </x14:formula1>
@@ -9869,15 +10024,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:L22"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9899,22 +10054,22 @@
   <sheetData>
     <row r="1" spans="1:12" s="8" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>1</v>
@@ -9929,36 +10084,36 @@
         <v>5</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E2" s="10">
         <v>44672</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="10"/>
@@ -9967,28 +10122,28 @@
     </row>
     <row r="3" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E3" s="10">
         <v>44672</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="10"/>
@@ -9997,28 +10152,28 @@
     </row>
     <row r="4" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E4" s="10">
         <v>44672</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="10"/>
@@ -10027,60 +10182,60 @@
     </row>
     <row r="5" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E5" s="10">
         <v>44672</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="10"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E6" s="10">
         <v>44672</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="10"/>
@@ -10089,13 +10244,13 @@
     </row>
     <row r="7" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>22</v>
@@ -10104,13 +10259,13 @@
         <v>44672</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="10"/>
@@ -10119,28 +10274,28 @@
     </row>
     <row r="8" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E8" s="10">
         <v>44672</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="10"/>
@@ -10149,28 +10304,28 @@
     </row>
     <row r="9" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E9" s="10">
         <v>44672</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="10"/>
@@ -10178,46 +10333,46 @@
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="37"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="41"/>
     </row>
     <row r="11" spans="1:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E11" s="10">
         <v>44686</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J11" s="10">
         <v>44686</v>
@@ -10227,31 +10382,31 @@
     </row>
     <row r="12" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E12" s="10">
         <v>44686</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J12" s="10">
         <v>44686</v>
@@ -10261,69 +10416,69 @@
     </row>
     <row r="13" spans="1:12" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E13" s="10">
         <v>44686</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J13" s="10">
         <v>44686</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E14" s="10">
         <v>44686</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J14" s="10">
         <v>44686</v>
@@ -10333,31 +10488,31 @@
     </row>
     <row r="15" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E15" s="10">
         <v>44686</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J15" s="10">
         <v>44686</v>
@@ -10367,69 +10522,69 @@
     </row>
     <row r="16" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E16" s="10">
         <v>44686</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J16" s="10">
         <v>44686</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E17" s="10">
         <v>44686</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J17" s="10">
         <v>44686</v>
@@ -10439,31 +10594,31 @@
     </row>
     <row r="18" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E18" s="10">
         <v>44686</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J18" s="10">
         <v>44686</v>
@@ -10473,65 +10628,67 @@
     </row>
     <row r="19" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E19" s="10">
         <v>44686</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J19" s="10">
         <v>44686</v>
       </c>
-      <c r="K19" s="6"/>
+      <c r="K19" s="6" t="s">
+        <v>203</v>
+      </c>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E20" s="10">
         <v>44686</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J20" s="10">
         <v>44686</v>
@@ -10541,226 +10698,669 @@
     </row>
     <row r="21" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E21" s="10">
         <v>44686</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J21" s="10">
         <v>44686</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" s="10">
         <v>44686</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J22" s="10">
         <v>44686</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="10">
+        <v>44686</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J23" s="10">
+        <v>44686</v>
+      </c>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="10">
+        <v>44686</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J24" s="10">
+        <v>44686</v>
+      </c>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="10">
+        <v>44686</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J25" s="10">
+        <v>44686</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="10">
+        <v>44686</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J26" s="10">
+        <v>44686</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="10">
+        <v>44686</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J27" s="10">
+        <v>44686</v>
+      </c>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="39"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="41"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="10">
+        <v>44688</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="H29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="10">
+        <v>44688</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="H30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="10">
+        <v>44688</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="H31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" s="10">
+        <v>44688</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="H32" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
-  <mergeCells count="1">
+  <autoFilter ref="A1:L1" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
+  <mergeCells count="2">
     <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A28:L28"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:H9">
-    <cfRule type="cellIs" dxfId="47" priority="85" operator="equal">
+  <conditionalFormatting sqref="H29:H1048576">
+    <cfRule type="cellIs" dxfId="91" priority="185" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="186" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="187" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="88" operator="equal">
-      <formula>"Open"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9 H23:H1048576">
-    <cfRule type="cellIs" dxfId="43" priority="81" operator="equal">
-      <formula>"Need Approval"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="82" operator="equal">
-      <formula>"In progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="83" operator="equal">
-      <formula>"Closed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="188" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="39" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="101" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="102" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="103" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="104" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="35" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="97" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="98" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="99" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="100" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H16">
-    <cfRule type="cellIs" dxfId="31" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="93" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="94" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="95" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="96" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H16">
-    <cfRule type="cellIs" dxfId="27" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="89" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="90" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="91" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="92" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="77" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="78" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="79" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="80" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="73" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="74" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="75" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="76" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="85" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="86" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="87" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="88" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="81" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="82" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="83" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="84" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
+    <cfRule type="cellIs" dxfId="55" priority="69" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="70" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="71" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="72" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="cellIs" dxfId="51" priority="65" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="66" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="67" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="68" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H9">
+    <cfRule type="cellIs" dxfId="47" priority="61" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="62" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="63" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="64" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H9">
+    <cfRule type="cellIs" dxfId="43" priority="57" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="58" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="59" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="60" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -10774,7 +11374,7 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
+  <conditionalFormatting sqref="H27">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -10792,12 +11392,18 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000000000000}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000000000000}">
           <x14:formula1>
             <xm:f>Options!$B$1:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H9 H11:H1048576</xm:sqref>
+          <xm:sqref>H29:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
+          <x14:formula1>
+            <xm:f>Options!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>H1:H9 H11:H27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10805,12 +11411,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A3:N46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10822,7 +11428,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="42" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -10830,9 +11436,9 @@
       </c>
       <c r="C3" s="3">
         <f>COUNTIFS(PMP_Review!F2:F1048576,"Open")</f>
-        <v>1</v>
-      </c>
-      <c r="L3" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="43" t="s">
         <v>10</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -10844,15 +11450,15 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3">
         <f>COUNTIFS(PMP_Review!F2:F1048576,"Closed")</f>
-        <v>13</v>
-      </c>
-      <c r="L4" s="39"/>
+        <v>14</v>
+      </c>
+      <c r="L4" s="43"/>
       <c r="M4" s="4" t="s">
         <v>6</v>
       </c>
@@ -10862,17 +11468,17 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="14">
         <f>COUNTIFS(PMP_Review!F2:F1048576,"In Progress")</f>
         <v>0</v>
       </c>
-      <c r="L5" s="39"/>
+      <c r="L5" s="43"/>
       <c r="M5" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N5" s="15">
         <f>COUNTIFS(SRS_Review!F2:F1048576,"In Progress")</f>
@@ -10880,17 +11486,17 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="14">
         <f>COUNTIFS(PMP_Review!F2:F1048576,"Need Approval")</f>
         <v>0</v>
       </c>
-      <c r="L6" s="39"/>
+      <c r="L6" s="43"/>
       <c r="M6" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N6" s="15">
         <f>COUNTIFS(SRS_Review!F2:F1048576,"Need Approval")</f>
@@ -10898,7 +11504,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -10906,7 +11512,7 @@
         <f>SUM(C3:C6)</f>
         <v>14</v>
       </c>
-      <c r="L7" s="39"/>
+      <c r="L7" s="43"/>
       <c r="M7" s="4" t="s">
         <v>9</v>
       </c>
@@ -10916,194 +11522,194 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="24" t="s">
+      <c r="A23" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="B23" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="24">
-        <f>COUNTIF(Scope_Statment_Review!F2:F1048576,"Open")</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="M23" s="25" t="s">
+      <c r="C23" s="23">
+        <f>COUNTIF(WireFrame_Review!F2:F1048576,"Open")</f>
+        <v>2</v>
+      </c>
+      <c r="L23" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="M23" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="N23" s="25">
+      <c r="N23" s="24">
         <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"Open")</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="24" t="s">
+      <c r="A24" s="42"/>
+      <c r="B24" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="24">
-        <f>COUNTIF(Scope_Statment_Review!F2:F1048576,"Closed")</f>
-        <v>2</v>
-      </c>
-      <c r="L24" s="39"/>
-      <c r="M24" s="25" t="s">
+      <c r="C24" s="23">
+        <f>COUNTIF(WireFrame_Review!F2:F1048576,"Closed")</f>
+        <v>10</v>
+      </c>
+      <c r="L24" s="43"/>
+      <c r="M24" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="N24" s="25">
+      <c r="N24" s="24">
         <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"Closed")</f>
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
-      <c r="B25" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="24">
-        <f>COUNTIF(Scope_Statment_Review!F2:F1048576,"In Progress")</f>
+      <c r="A25" s="42"/>
+      <c r="B25" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="23">
+        <f>COUNTIF(WireFrame_Review!F2:F1048576,"In Progress")</f>
         <v>0</v>
       </c>
-      <c r="L25" s="39"/>
-      <c r="M25" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="N25" s="25">
+      <c r="L25" s="43"/>
+      <c r="M25" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="N25" s="24">
         <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"In Progress")</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="38"/>
-      <c r="B26" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="24">
-        <f>COUNTIF(Scope_Statment_Review!F2:F1048576,"Need Approval")</f>
+      <c r="A26" s="42"/>
+      <c r="B26" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="23">
+        <f>COUNTIF(WireFrame_Review!F2:F1048576,"Need Approval")</f>
         <v>0</v>
       </c>
-      <c r="L26" s="39"/>
-      <c r="M26" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="N26" s="25">
+      <c r="L26" s="43"/>
+      <c r="M26" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="N26" s="24">
         <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"Need Approval")</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="38"/>
-      <c r="B27" s="24" t="s">
+      <c r="A27" s="42"/>
+      <c r="B27" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="23">
         <f>SUM(C23:C26)</f>
-        <v>2</v>
-      </c>
-      <c r="L27" s="39"/>
-      <c r="M27" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="43"/>
+      <c r="M27" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="N27" s="25">
+      <c r="N27" s="24">
         <f>SUM(N23:N26)</f>
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="H34" s="26"/>
+      <c r="H34" s="25"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="B42" s="24" t="s">
+      <c r="A42" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="24">
+      <c r="C42" s="23">
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Open")</f>
         <v>0</v>
       </c>
-      <c r="L42" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="M42" s="25" t="s">
+      <c r="L42" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="M42" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="N42" s="25">
+      <c r="N42" s="24">
         <f>COUNTIF(Audit_Review!H2:H1048576,"Open")</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" s="38"/>
-      <c r="B43" s="24" t="s">
+      <c r="A43" s="42"/>
+      <c r="B43" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="24">
+      <c r="C43" s="23">
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Closed")</f>
         <v>2</v>
       </c>
-      <c r="L43" s="39"/>
-      <c r="M43" s="25" t="s">
+      <c r="L43" s="43"/>
+      <c r="M43" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="N43" s="25">
+      <c r="N43" s="24">
         <f>COUNTIF(Audit_Review!H2:H1048576,"Closed")</f>
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" s="38"/>
-      <c r="B44" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="24">
+      <c r="A44" s="42"/>
+      <c r="B44" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="23">
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"In Progress")</f>
         <v>0</v>
       </c>
-      <c r="L44" s="39"/>
-      <c r="M44" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="N44" s="25">
+      <c r="L44" s="43"/>
+      <c r="M44" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="N44" s="24">
         <f>COUNTIF(Audit_Review!H2:H1048576,"In Progress")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" s="38"/>
-      <c r="B45" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C45" s="24">
+      <c r="A45" s="42"/>
+      <c r="B45" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="23">
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Need Approval")</f>
         <v>0</v>
       </c>
-      <c r="L45" s="39"/>
-      <c r="M45" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="N45" s="25">
+      <c r="L45" s="43"/>
+      <c r="M45" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="N45" s="24">
         <f>COUNTIF(Audit_Review!H2:H1048576,"Need Approval")</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" s="38"/>
-      <c r="B46" s="24" t="s">
+      <c r="A46" s="42"/>
+      <c r="B46" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="24">
+      <c r="C46" s="23">
         <f>SUM(C42:C45)</f>
         <v>2</v>
       </c>
-      <c r="L46" s="39"/>
-      <c r="M46" s="25" t="s">
+      <c r="L46" s="43"/>
+      <c r="M46" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="N46" s="25">
+      <c r="N46" s="24">
         <f>SUM(N42:N45)</f>
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ERD reviews are approved and closed
</commit_message>
<xml_diff>
--- a/Monitor and Control/F_Review.xlsx
+++ b/Monitor and Control/F_Review.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_903702A62FB51BCEC4DBA4FAF014D795A3CCA902" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6998E0C0-D2BC-40AB-92AB-ABB6DC20C73B}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_903702A62FB51BCEC4DBA4FAF014D795A3CCA902" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{607EF988-7EB6-405C-9F86-E471132EFCB4}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="2508" windowWidth="17280" windowHeight="8880" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP_Review" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="237">
   <si>
     <t>Raised By</t>
   </si>
@@ -9479,8 +9479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A3CFC9-F983-492B-BEA4-AEE18E86BD58}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9546,10 +9546,14 @@
         <v>235</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="10">
+        <v>44690</v>
+      </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
     </row>
@@ -9570,10 +9574,14 @@
         <v>236</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H3" s="10">
+        <v>44690</v>
+      </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
@@ -9801,30 +9809,30 @@
     <mergeCell ref="B13:J13"/>
   </mergeCells>
   <conditionalFormatting sqref="F14:F21 F32:F38 F1:F2 F40:F1048576 F4:F12">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10453,16 +10461,16 @@
     <mergeCell ref="B13:J13"/>
   </mergeCells>
   <conditionalFormatting sqref="F14:F21 F32:F38 F1:F12 F40:F1048576">
-    <cfRule type="cellIs" dxfId="107" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10656,16 +10664,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F14:F21 F23:F1048576 F1:F12">
-    <cfRule type="cellIs" dxfId="103" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11728,324 +11736,324 @@
     <mergeCell ref="A28:L28"/>
   </mergeCells>
   <conditionalFormatting sqref="H29:H1048576">
-    <cfRule type="cellIs" dxfId="99" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="185" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="186" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="187" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="188" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="95" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="101" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="102" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="103" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="104" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="91" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="97" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="98" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="99" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="100" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H16">
-    <cfRule type="cellIs" dxfId="87" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="93" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="94" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="95" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="96" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H16">
-    <cfRule type="cellIs" dxfId="83" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="89" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="90" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="91" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="92" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="79" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="77" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="78" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="79" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="80" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="75" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="73" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="74" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="75" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="76" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="71" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="85" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="86" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="87" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="88" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="67" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="81" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="82" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="83" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="84" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="63" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="69" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="70" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="71" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="72" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="59" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="65" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="66" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="67" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="68" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="cellIs" dxfId="55" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="61" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="62" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="63" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="64" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H9">
-    <cfRule type="cellIs" dxfId="51" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="57" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="58" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="59" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="60" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="35" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
implementation review register/login/add admin/add user
</commit_message>
<xml_diff>
--- a/Monitor and Control/F_Review.xlsx
+++ b/Monitor and Control/F_Review.xlsx
@@ -4,20 +4,24 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PMP_Review" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="5" state="hidden" r:id="rId2"/>
     <sheet name="Risk_Managment_Plan_Review" sheetId="7" r:id="rId3"/>
     <sheet name="WireFrame_Review" sheetId="12" r:id="rId4"/>
-    <sheet name="SRS_Review" sheetId="3" r:id="rId5"/>
-    <sheet name="Sequence_Diagrams_Review" sheetId="10" r:id="rId6"/>
-    <sheet name="Audit_Review" sheetId="11" r:id="rId7"/>
-    <sheet name="Progress_Chart" sheetId="4" r:id="rId8"/>
+    <sheet name="Implementation_Review" sheetId="13" r:id="rId5"/>
+    <sheet name="SRS_Review" sheetId="3" r:id="rId6"/>
+    <sheet name="Sequence_Diagrams_Review" sheetId="10" r:id="rId7"/>
+    <sheet name="Audit_Review" sheetId="11" r:id="rId8"/>
+    <sheet name="Progress_Chart" sheetId="4" r:id="rId9"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId10"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Audit_Review!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Audit_Review!$A$1:$L$1</definedName>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="248">
   <si>
     <t>Raised By</t>
   </si>
@@ -755,6 +759,91 @@
       <t xml:space="preserve"> NOTE: This is the nav bar after the user signs in. "Register and "Sign out" buttons will take place the "Sign out" button in the nav bar if the user has not registered or signed in.</t>
     </r>
   </si>
+  <si>
+    <t>F_REVIEW_register_001</t>
+  </si>
+  <si>
+    <t>13/5</t>
+  </si>
+  <si>
+    <r>
+      <t>according srs and sequence all error messages must be appear after user click "register "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>button</t>
+    </r>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>F_REVIEW_register_002</t>
+  </si>
+  <si>
+    <t>fullname&amp;username accept numbers</t>
+  </si>
+  <si>
+    <t>F_REVIEW_register_003</t>
+  </si>
+  <si>
+    <t>phone number accept characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Already a member? LogIn must be replace with 
+“Have an account? Login here”. </t>
+  </si>
+  <si>
+    <t>F_REVIEW_login_001</t>
+  </si>
+  <si>
+    <t>F_REVIEW_AddAdmin_001</t>
+  </si>
+  <si>
+    <t>check vaildation of all fields in add admin page</t>
+  </si>
+  <si>
+    <t>F_REVIEW_AddAdmin_002</t>
+  </si>
+  <si>
+    <t>Add Admin button replace with Add</t>
+  </si>
+  <si>
+    <t>F_REVIEW_AddUser_001</t>
+  </si>
+  <si>
+    <t>Add User button replace with Add</t>
+  </si>
+  <si>
+    <t>F_REVIEW_AddUser_002</t>
+  </si>
+  <si>
+    <t>username accept numbers must be characters only so an error
+ message will appear saying that “Invalid username or password”after click login</t>
+  </si>
+  <si>
+    <t>Hagar Nasser</t>
+  </si>
+  <si>
+    <t>replace useremail with email(wirefram)</t>
+  </si>
 </sst>
 </file>
 
@@ -763,7 +852,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -780,6 +869,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1019,7 +1116,35 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="176">
+  <dxfs count="180">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3668,7 +3793,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>17</c:v>
@@ -7614,6 +7739,35 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="PMP_Review"/>
+      <sheetName val="Options"/>
+      <sheetName val="Risk_Managment_Plan_Review"/>
+      <sheetName val="WireFrame_Review"/>
+      <sheetName val="ERD_Review"/>
+      <sheetName val="SRS_Review"/>
+      <sheetName val="Sequence_Diagrams_Review"/>
+      <sheetName val="Audit_Review"/>
+      <sheetName val="Progress_Chart"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7886,20 +8040,20 @@
       <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="71.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="71.109375" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>172</v>
       </c>
@@ -7931,7 +8085,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>78</v>
       </c>
@@ -7959,7 +8113,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>79</v>
       </c>
@@ -7987,7 +8141,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -8015,7 +8169,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>81</v>
       </c>
@@ -8043,7 +8197,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>82</v>
       </c>
@@ -8071,7 +8225,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>83</v>
       </c>
@@ -8099,7 +8253,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="34"/>
       <c r="C8" s="35"/>
@@ -8111,7 +8265,7 @@
       <c r="I8" s="35"/>
       <c r="J8" s="36"/>
     </row>
-    <row r="9" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>92</v>
       </c>
@@ -8139,7 +8293,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>93</v>
       </c>
@@ -8167,7 +8321,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>94</v>
       </c>
@@ -8199,7 +8353,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>95</v>
       </c>
@@ -8227,7 +8381,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>96</v>
       </c>
@@ -8255,7 +8409,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>97</v>
       </c>
@@ -8283,7 +8437,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>98</v>
       </c>
@@ -8311,7 +8465,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="34"/>
       <c r="C16" s="35"/>
@@ -8323,7 +8477,7 @@
       <c r="I16" s="35"/>
       <c r="J16" s="36"/>
     </row>
-    <row r="17" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>99</v>
       </c>
@@ -8357,44 +8511,44 @@
     <mergeCell ref="B16:J16"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F15 F18:F1048576">
-    <cfRule type="cellIs" dxfId="175" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="10" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="171" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="6" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="167" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8423,27 +8577,27 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>66</v>
       </c>
@@ -8464,21 +8618,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="62.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="62.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
     <col min="9" max="9" width="34" style="16" customWidth="1"/>
-    <col min="10" max="10" width="32.28515625" style="16" customWidth="1"/>
+    <col min="10" max="10" width="32.33203125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>172</v>
       </c>
@@ -8510,7 +8664,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>68</v>
       </c>
@@ -8538,7 +8692,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>69</v>
       </c>
@@ -8566,7 +8720,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>70</v>
       </c>
@@ -8594,7 +8748,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>71</v>
       </c>
@@ -8626,7 +8780,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>72</v>
       </c>
@@ -8654,7 +8808,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>73</v>
       </c>
@@ -8684,16 +8838,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="163" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8716,28 +8870,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="54" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="34.7109375" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="9"/>
+    <col min="6" max="6" width="13.88671875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="34.6640625" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>172</v>
       </c>
@@ -8769,7 +8923,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>173</v>
       </c>
@@ -8795,7 +8949,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="122.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>174</v>
       </c>
@@ -8821,7 +8975,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" s="33" customFormat="1" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="33" customFormat="1" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>178</v>
       </c>
@@ -8845,7 +8999,7 @@
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
     </row>
-    <row r="5" spans="1:10" s="33" customFormat="1" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="33" customFormat="1" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>181</v>
       </c>
@@ -8871,7 +9025,7 @@
       <c r="I5" s="28"/>
       <c r="J5" s="28"/>
     </row>
-    <row r="6" spans="1:10" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>182</v>
       </c>
@@ -8897,7 +9051,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>183</v>
       </c>
@@ -8923,7 +9077,7 @@
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
     </row>
-    <row r="8" spans="1:10" s="33" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="33" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>185</v>
       </c>
@@ -8949,7 +9103,7 @@
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
     </row>
-    <row r="9" spans="1:10" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>187</v>
       </c>
@@ -8975,7 +9129,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>190</v>
       </c>
@@ -9001,7 +9155,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>192</v>
       </c>
@@ -9027,7 +9181,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>194</v>
       </c>
@@ -9053,7 +9207,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>196</v>
       </c>
@@ -9079,7 +9233,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="34"/>
       <c r="B14" s="35"/>
       <c r="C14" s="35"/>
@@ -9091,7 +9245,7 @@
       <c r="I14" s="35"/>
       <c r="J14" s="36"/>
     </row>
-    <row r="15" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>216</v>
       </c>
@@ -9117,7 +9271,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>218</v>
       </c>
@@ -9143,7 +9297,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>220</v>
       </c>
@@ -9169,7 +9323,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>222</v>
       </c>
@@ -9195,7 +9349,7 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>224</v>
       </c>
@@ -9221,233 +9375,256 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D20" s="7"/>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D21" s="7"/>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D22" s="7"/>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D23" s="7"/>
-      <c r="E23" s="11"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="34"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="36"/>
+    </row>
+    <row r="21" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" t="s">
+        <v>246</v>
+      </c>
+      <c r="D21" t="s">
+        <v>229</v>
+      </c>
+      <c r="E21" t="s">
+        <v>247</v>
+      </c>
+      <c r="F21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" t="s">
+        <v>246</v>
+      </c>
+      <c r="D22" t="s">
+        <v>229</v>
+      </c>
+      <c r="E22" t="s">
+        <v>247</v>
+      </c>
+      <c r="F22" t="s">
+        <v>231</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A20:J20"/>
   </mergeCells>
-  <conditionalFormatting sqref="F24:F1048576 F1:F3">
-    <cfRule type="cellIs" dxfId="159" priority="65" operator="equal">
+  <conditionalFormatting sqref="F23:F1048576 F1:F3">
+    <cfRule type="cellIs" dxfId="163" priority="65" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="66" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="67" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="68" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="155" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="61" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="62" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="63" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="64" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="151" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="57" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="58" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="59" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="60" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="147" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="53" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="54" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="55" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="56" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="143" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="49" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="50" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="51" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="52" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="139" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="45" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="46" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="47" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="48" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="135" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="41" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="42" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="43" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="44" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="131" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="37" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="38" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="39" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="40" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="127" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="33" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="34" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="35" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="36" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="123" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="29" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="30" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="31" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="32" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="119" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="25" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="26" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="27" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="28" operator="equal">
-      <formula>"Open"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F23">
-    <cfRule type="cellIs" dxfId="115" priority="21" operator="equal">
-      <formula>"Need Approval"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="22" operator="equal">
-      <formula>"In progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="23" operator="equal">
-      <formula>"Closed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="28" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="111" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="107" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:F19">
-    <cfRule type="cellIs" dxfId="103" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9460,7 +9637,7 @@
           <x14:formula1>
             <xm:f>Options!$B$1:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
+          <xm:sqref>F1:F20 F23:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9469,6 +9646,272 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="39.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="F2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="F5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" t="s">
+        <v>239</v>
+      </c>
+      <c r="F9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D10" t="s">
+        <v>229</v>
+      </c>
+      <c r="E10" t="s">
+        <v>241</v>
+      </c>
+      <c r="F10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12" t="s">
+        <v>229</v>
+      </c>
+      <c r="E12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" t="s">
+        <v>229</v>
+      </c>
+      <c r="E13" t="s">
+        <v>239</v>
+      </c>
+      <c r="F13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F1">
+    <cfRule type="cellIs" dxfId="103" priority="1" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="2" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="3" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="4" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'F:\monika\QA_Foodies\Monitor and Control\[F_Review.xlsx]Options'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>F1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
@@ -9479,21 +9922,21 @@
       <selection pane="bottomRight" activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="88.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="88.44140625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>172</v>
       </c>
@@ -9525,7 +9968,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>47</v>
       </c>
@@ -9553,7 +9996,7 @@
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
     </row>
-    <row r="3" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>48</v>
       </c>
@@ -9581,7 +10024,7 @@
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>49</v>
       </c>
@@ -9609,7 +10052,7 @@
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>50</v>
       </c>
@@ -9637,7 +10080,7 @@
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>51</v>
       </c>
@@ -9665,7 +10108,7 @@
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>52</v>
       </c>
@@ -9693,7 +10136,7 @@
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>53</v>
       </c>
@@ -9721,7 +10164,7 @@
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>54</v>
       </c>
@@ -9749,7 +10192,7 @@
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
     </row>
-    <row r="10" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>55</v>
       </c>
@@ -9777,7 +10220,7 @@
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>56</v>
       </c>
@@ -9805,7 +10248,7 @@
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="1:10" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -9833,7 +10276,7 @@
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="34"/>
       <c r="C13" s="35"/>
@@ -9845,7 +10288,7 @@
       <c r="I13" s="35"/>
       <c r="J13" s="36"/>
     </row>
-    <row r="14" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>58</v>
       </c>
@@ -9873,7 +10316,7 @@
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
     </row>
-    <row r="15" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>59</v>
       </c>
@@ -9901,7 +10344,7 @@
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
     </row>
-    <row r="16" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>60</v>
       </c>
@@ -9929,7 +10372,7 @@
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
     </row>
-    <row r="17" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>61</v>
       </c>
@@ -9957,7 +10400,7 @@
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
     </row>
-    <row r="18" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>62</v>
       </c>
@@ -9985,7 +10428,7 @@
       <c r="I18" s="17"/>
       <c r="J18" s="17"/>
     </row>
-    <row r="19" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>63</v>
       </c>
@@ -10013,7 +10456,7 @@
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
     </row>
-    <row r="20" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>64</v>
       </c>
@@ -10041,7 +10484,7 @@
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
     </row>
-    <row r="21" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>65</v>
       </c>
@@ -10069,7 +10512,7 @@
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F39"/>
     </row>
   </sheetData>
@@ -10107,7 +10550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
@@ -10115,21 +10558,21 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="34.7109375" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="50.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="34.6640625" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>172</v>
       </c>
@@ -10161,7 +10604,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>104</v>
       </c>
@@ -10191,7 +10634,7 @@
       </c>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>105</v>
       </c>
@@ -10221,61 +10664,61 @@
       </c>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F10" s="21"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F11" s="21"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F17" s="21"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F18" s="21"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F19" s="21"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F21" s="21"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F22"/>
     </row>
   </sheetData>
@@ -10309,7 +10752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
@@ -10320,24 +10763,24 @@
       <selection pane="bottomRight" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" customWidth="1"/>
+    <col min="11" max="11" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.6640625" customWidth="1"/>
     <col min="13" max="13" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>172</v>
       </c>
@@ -10375,7 +10818,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>112</v>
       </c>
@@ -10405,7 +10848,7 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>113</v>
       </c>
@@ -10435,7 +10878,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>118</v>
       </c>
@@ -10465,7 +10908,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>120</v>
       </c>
@@ -10497,7 +10940,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>121</v>
       </c>
@@ -10527,7 +10970,7 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>126</v>
       </c>
@@ -10557,7 +11000,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>127</v>
       </c>
@@ -10587,7 +11030,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>133</v>
       </c>
@@ -10617,7 +11060,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
@@ -10631,7 +11074,7 @@
       <c r="K10" s="38"/>
       <c r="L10" s="39"/>
     </row>
-    <row r="11" spans="1:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>135</v>
       </c>
@@ -10665,7 +11108,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>145</v>
       </c>
@@ -10699,7 +11142,7 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>149</v>
       </c>
@@ -10737,7 +11180,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>151</v>
       </c>
@@ -10771,7 +11214,7 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>152</v>
       </c>
@@ -10805,7 +11248,7 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>154</v>
       </c>
@@ -10843,7 +11286,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>160</v>
       </c>
@@ -10877,7 +11320,7 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>161</v>
       </c>
@@ -10911,7 +11354,7 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>162</v>
       </c>
@@ -10947,7 +11390,7 @@
       </c>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>166</v>
       </c>
@@ -10981,7 +11424,7 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>168</v>
       </c>
@@ -11019,7 +11462,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>170</v>
       </c>
@@ -11057,7 +11500,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>200</v>
       </c>
@@ -11091,7 +11534,7 @@
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>202</v>
       </c>
@@ -11125,7 +11568,7 @@
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>203</v>
       </c>
@@ -11159,7 +11602,7 @@
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>206</v>
       </c>
@@ -11193,7 +11636,7 @@
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>207</v>
       </c>
@@ -11227,7 +11670,7 @@
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" s="38"/>
       <c r="C28" s="38"/>
@@ -11241,7 +11684,7 @@
       <c r="K28" s="38"/>
       <c r="L28" s="39"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
         <v>208</v>
       </c>
@@ -11267,7 +11710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="29" t="s">
         <v>212</v>
       </c>
@@ -11293,7 +11736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="29" t="s">
         <v>213</v>
       </c>
@@ -11319,7 +11762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="29" t="s">
         <v>214</v>
       </c>
@@ -11696,7 +12139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N46"/>
   <sheetViews>
@@ -11704,15 +12147,15 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>8</v>
       </c>
@@ -11734,7 +12177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="40"/>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -11752,7 +12195,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="40"/>
       <c r="B5" s="14" t="s">
         <v>46</v>
@@ -11770,7 +12213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="40"/>
       <c r="B6" s="14" t="s">
         <v>66</v>
@@ -11788,7 +12231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="40"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -11806,7 +12249,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="40" t="s">
         <v>199</v>
       </c>
@@ -11815,7 +12258,7 @@
       </c>
       <c r="C23" s="23">
         <f>COUNTIF(WireFrame_Review!F2:F1048576,"Open")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23" s="41" t="s">
         <v>76</v>
@@ -11828,7 +12271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="40"/>
       <c r="B24" s="23" t="s">
         <v>6</v>
@@ -11846,7 +12289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="40"/>
       <c r="B25" s="23" t="s">
         <v>46</v>
@@ -11864,7 +12307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="40"/>
       <c r="B26" s="23" t="s">
         <v>66</v>
@@ -11882,14 +12325,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="40"/>
       <c r="B27" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="23">
         <f>SUM(C23:C26)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L27" s="41"/>
       <c r="M27" s="24" t="s">
@@ -11900,10 +12343,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H34" s="25"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="40" t="s">
         <v>111</v>
       </c>
@@ -11925,7 +12368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="40"/>
       <c r="B43" s="23" t="s">
         <v>6</v>
@@ -11943,7 +12386,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="40"/>
       <c r="B44" s="23" t="s">
         <v>46</v>
@@ -11961,7 +12404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="40"/>
       <c r="B45" s="23" t="s">
         <v>66</v>
@@ -11979,7 +12422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="40"/>
       <c r="B46" s="23" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Issue in the SRS
</commit_message>
<xml_diff>
--- a/Monitor and Control/F_Review.xlsx
+++ b/Monitor and Control/F_Review.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="16" documentId="14_{9DCE3201-9654-4435-99AF-AD045B2B1C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E7E78FB-30E2-4D03-B4F9-F546B3CCB6CA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BF1A2C-4FD9-4842-BF77-49E0CF1BD669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP_Review" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Audit_Review!$A$1:$L$1</definedName>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,9 +33,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -45,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="260">
   <si>
     <t>Raised By</t>
   </si>
@@ -877,6 +875,12 @@
   </si>
   <si>
     <t>Validation is added and this issue is resolved.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_SRS_V1.2_020</t>
+  </si>
+  <si>
+    <t>change the discount amount in offers to be float not interger</t>
   </si>
 </sst>
 </file>
@@ -967,7 +971,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1047,12 +1051,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1141,6 +1167,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1165,25 +1212,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1191,91 +1238,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="228">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="216">
     <dxf>
       <fill>
         <patternFill>
@@ -3208,7 +3171,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>19</c:v>
@@ -8666,15 +8629,15 @@
     </row>
     <row r="8" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="36"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
     </row>
     <row r="9" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
@@ -8878,15 +8841,15 @@
     </row>
     <row r="16" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="36"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="43"/>
     </row>
     <row r="17" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
@@ -8922,44 +8885,44 @@
     <mergeCell ref="B16:J16"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F15 F18:F1048576">
-    <cfRule type="cellIs" dxfId="227" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="10" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="224" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="223" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="6" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="219" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9249,16 +9212,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="215" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9647,16 +9610,16 @@
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="36"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
@@ -9789,16 +9752,16 @@
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="34"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="36"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="43"/>
     </row>
     <row r="21" spans="1:10" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
@@ -9852,240 +9815,240 @@
     <mergeCell ref="A20:J20"/>
   </mergeCells>
   <conditionalFormatting sqref="F23:F1048576 F1:F3">
-    <cfRule type="cellIs" dxfId="211" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="77" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="78" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="79" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="80" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="207" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="73" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="74" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="75" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="76" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="203" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="69" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="70" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="71" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="72" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="199" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="65" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="66" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="67" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="68" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="195" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="61" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="62" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="63" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="64" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="191" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="57" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="58" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="59" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="60" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="187" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="53" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="54" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="55" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="56" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="183" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="49" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="50" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="51" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="52" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="179" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="45" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="46" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="47" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="48" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="175" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="41" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="42" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="43" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="44" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="171" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="37" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="38" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="39" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="40" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="167" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="21" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="22" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="23" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="163" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="17" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="18" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="19" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:F19">
-    <cfRule type="cellIs" dxfId="159" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="14" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="15" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21 H21">
-    <cfRule type="cellIs" dxfId="51" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="47" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10110,291 +10073,291 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C4" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" style="46" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="46" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="46" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" style="46" customWidth="1"/>
-    <col min="5" max="16384" width="50.5546875" style="46"/>
+    <col min="1" max="1" width="37.33203125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" style="38" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" style="38" customWidth="1"/>
+    <col min="5" max="16384" width="50.5546875" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="44" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:10" s="36" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="34" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="39" t="s">
         <v>253</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="39" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="37" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="38" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="38" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+    <row r="5" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="38" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:10" ht="78" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
+    <row r="6" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="39" t="s">
         <v>243</v>
       </c>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="38" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:10" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="37" t="s">
         <v>236</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="I9" s="46" t="s">
+      <c r="I9" s="38" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="37" t="s">
         <v>238</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="F10" s="48" t="s">
+      <c r="F10" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="38" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="F12" s="48" t="s">
+      <c r="F12" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="46" t="s">
+      <c r="H12" s="38" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E13" s="46" t="s">
+      <c r="E13" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="F13" s="48" t="s">
+      <c r="F13" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="46" t="s">
+      <c r="H13" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="I13" s="46" t="s">
+      <c r="I13" s="38" t="s">
         <v>257</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="155" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10419,11 +10382,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22:XFD22"/>
+      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10782,15 +10745,15 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="36"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="43"/>
     </row>
     <row r="14" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
@@ -11016,24 +10979,65 @@
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
     </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="43"/>
+    </row>
+    <row r="24" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="53" t="s">
+        <v>258</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="55" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" s="49">
+        <v>44700</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>259</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="51"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="21"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="49"/>
+    </row>
     <row r="39" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F39"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B23:J23"/>
   </mergeCells>
   <conditionalFormatting sqref="F14:F21 F32:F38 F1:F12 F40:F1048576">
-    <cfRule type="cellIs" dxfId="151" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11227,16 +11231,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F14:F21 F23:F1048576 F1:F12">
-    <cfRule type="cellIs" dxfId="147" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11566,18 +11570,18 @@
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="46"/>
     </row>
     <row r="11" spans="1:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -12176,18 +12180,18 @@
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="37"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="39"/>
+      <c r="A28" s="44"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="46"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
@@ -12324,282 +12328,282 @@
     <mergeCell ref="A28:L28"/>
   </mergeCells>
   <conditionalFormatting sqref="H33:H1048576">
-    <cfRule type="cellIs" dxfId="143" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="225" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="226" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="227" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="227" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="228" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="139" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="141" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="142" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="143" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="144" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="135" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="137" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="138" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="139" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="140" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H16">
-    <cfRule type="cellIs" dxfId="131" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="133" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="134" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="135" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="136" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H16">
-    <cfRule type="cellIs" dxfId="127" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="129" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="130" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="131" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="132" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="115" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="125" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="126" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="127" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="128" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="111" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="121" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="122" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="123" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="124" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="107" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="109" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="110" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="111" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="112" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="103" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="105" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="106" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="107" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="108" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="99" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="101" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="102" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="103" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="104" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="91" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="77" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="78" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="79" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="80" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="87" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="73" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="74" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="76" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="83" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="69" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="70" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="71" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="79" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="65" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="68" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="75" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="61" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="62" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="63" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="64" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="71" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="59" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="67" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="53" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="63" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="59" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="55" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12783,7 +12787,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="47" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -12793,7 +12797,7 @@
         <f>COUNTIFS(PMP_Review!F2:F1048576,"Open")</f>
         <v>0</v>
       </c>
-      <c r="L3" s="41" t="s">
+      <c r="L3" s="48" t="s">
         <v>10</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -12801,11 +12805,11 @@
       </c>
       <c r="N3" s="4">
         <f>COUNTIFS(SRS_Review!F2:F1048576,"Open")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -12813,7 +12817,7 @@
         <f>COUNTIFS(PMP_Review!F2:F1048576,"Closed")</f>
         <v>14</v>
       </c>
-      <c r="L4" s="41"/>
+      <c r="L4" s="48"/>
       <c r="M4" s="4" t="s">
         <v>6</v>
       </c>
@@ -12823,7 +12827,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="14" t="s">
         <v>46</v>
       </c>
@@ -12831,7 +12835,7 @@
         <f>COUNTIFS(PMP_Review!F2:F1048576,"In Progress")</f>
         <v>0</v>
       </c>
-      <c r="L5" s="41"/>
+      <c r="L5" s="48"/>
       <c r="M5" s="15" t="s">
         <v>46</v>
       </c>
@@ -12841,7 +12845,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="14" t="s">
         <v>66</v>
       </c>
@@ -12849,7 +12853,7 @@
         <f>COUNTIFS(PMP_Review!F2:F1048576,"Need Approval")</f>
         <v>0</v>
       </c>
-      <c r="L6" s="41"/>
+      <c r="L6" s="48"/>
       <c r="M6" s="15" t="s">
         <v>66</v>
       </c>
@@ -12859,7 +12863,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -12867,17 +12871,17 @@
         <f>SUM(C3:C6)</f>
         <v>14</v>
       </c>
-      <c r="L7" s="41"/>
+      <c r="L7" s="48"/>
       <c r="M7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="N7" s="4">
         <f>SUM(N3:N6)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="47" t="s">
         <v>199</v>
       </c>
       <c r="B23" s="23" t="s">
@@ -12887,7 +12891,7 @@
         <f>COUNTIF(WireFrame_Review!F2:F1048576,"Open")</f>
         <v>0</v>
       </c>
-      <c r="L23" s="41" t="s">
+      <c r="L23" s="48" t="s">
         <v>76</v>
       </c>
       <c r="M23" s="24" t="s">
@@ -12899,7 +12903,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="40"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="23" t="s">
         <v>6</v>
       </c>
@@ -12907,7 +12911,7 @@
         <f>COUNTIF(WireFrame_Review!F2:F1048576,"Closed")</f>
         <v>19</v>
       </c>
-      <c r="L24" s="41"/>
+      <c r="L24" s="48"/>
       <c r="M24" s="24" t="s">
         <v>6</v>
       </c>
@@ -12917,7 +12921,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="40"/>
+      <c r="A25" s="47"/>
       <c r="B25" s="23" t="s">
         <v>46</v>
       </c>
@@ -12925,7 +12929,7 @@
         <f>COUNTIF(WireFrame_Review!F2:F1048576,"In Progress")</f>
         <v>0</v>
       </c>
-      <c r="L25" s="41"/>
+      <c r="L25" s="48"/>
       <c r="M25" s="24" t="s">
         <v>46</v>
       </c>
@@ -12935,7 +12939,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="40"/>
+      <c r="A26" s="47"/>
       <c r="B26" s="23" t="s">
         <v>66</v>
       </c>
@@ -12943,7 +12947,7 @@
         <f>COUNTIF(WireFrame_Review!F2:F1048576,"Need Approval")</f>
         <v>0</v>
       </c>
-      <c r="L26" s="41"/>
+      <c r="L26" s="48"/>
       <c r="M26" s="24" t="s">
         <v>66</v>
       </c>
@@ -12953,7 +12957,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="40"/>
+      <c r="A27" s="47"/>
       <c r="B27" s="23" t="s">
         <v>9</v>
       </c>
@@ -12961,7 +12965,7 @@
         <f>SUM(C23:C26)</f>
         <v>19</v>
       </c>
-      <c r="L27" s="41"/>
+      <c r="L27" s="48"/>
       <c r="M27" s="24" t="s">
         <v>9</v>
       </c>
@@ -12974,7 +12978,7 @@
       <c r="H34" s="25"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="47" t="s">
         <v>111</v>
       </c>
       <c r="B42" s="23" t="s">
@@ -12984,7 +12988,7 @@
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Open")</f>
         <v>0</v>
       </c>
-      <c r="L42" s="41" t="s">
+      <c r="L42" s="48" t="s">
         <v>129</v>
       </c>
       <c r="M42" s="24" t="s">
@@ -12996,7 +13000,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" s="40"/>
+      <c r="A43" s="47"/>
       <c r="B43" s="23" t="s">
         <v>6</v>
       </c>
@@ -13004,7 +13008,7 @@
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Closed")</f>
         <v>2</v>
       </c>
-      <c r="L43" s="41"/>
+      <c r="L43" s="48"/>
       <c r="M43" s="24" t="s">
         <v>6</v>
       </c>
@@ -13014,7 +13018,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" s="40"/>
+      <c r="A44" s="47"/>
       <c r="B44" s="23" t="s">
         <v>46</v>
       </c>
@@ -13022,7 +13026,7 @@
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"In Progress")</f>
         <v>0</v>
       </c>
-      <c r="L44" s="41"/>
+      <c r="L44" s="48"/>
       <c r="M44" s="24" t="s">
         <v>46</v>
       </c>
@@ -13032,7 +13036,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" s="40"/>
+      <c r="A45" s="47"/>
       <c r="B45" s="23" t="s">
         <v>66</v>
       </c>
@@ -13040,7 +13044,7 @@
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Need Approval")</f>
         <v>0</v>
       </c>
-      <c r="L45" s="41"/>
+      <c r="L45" s="48"/>
       <c r="M45" s="24" t="s">
         <v>66</v>
       </c>
@@ -13050,7 +13054,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" s="40"/>
+      <c r="A46" s="47"/>
       <c r="B46" s="23" t="s">
         <v>9</v>
       </c>
@@ -13058,7 +13062,7 @@
         <f>SUM(C42:C45)</f>
         <v>2</v>
       </c>
-      <c r="L46" s="41"/>
+      <c r="L46" s="48"/>
       <c r="M46" s="24" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Added review on test cases of noura
</commit_message>
<xml_diff>
--- a/Monitor and Control/F_Review.xlsx
+++ b/Monitor and Control/F_Review.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E159D18-4CAE-433C-B33C-39F62B59F17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2E159D18-4CAE-433C-B33C-39F62B59F17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08C787AD-37C4-43F9-BA46-9C66560AA454}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP_Review" sheetId="1" r:id="rId1"/>
@@ -16,16 +16,17 @@
     <sheet name="SRS_Review" sheetId="3" r:id="rId6"/>
     <sheet name="Sequence_Diagrams_Review" sheetId="10" r:id="rId7"/>
     <sheet name="Audit_Review" sheetId="11" r:id="rId8"/>
-    <sheet name="Progress_Chart" sheetId="4" r:id="rId9"/>
+    <sheet name="TestCase_Part1_Review" sheetId="14" r:id="rId9"/>
+    <sheet name="Progress_Chart" sheetId="4" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Audit_Review!$A$1:$L$1</definedName>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="318">
   <si>
     <t>Raised By</t>
   </si>
@@ -941,6 +944,131 @@
   </si>
   <si>
     <t xml:space="preserve">Remove the pop of the login successfully </t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddOffer_TC_V1.0_001</t>
+  </si>
+  <si>
+    <t>Noura Amr</t>
+  </si>
+  <si>
+    <t>26/5/2022</t>
+  </si>
+  <si>
+    <t>In the testcases steps, write only the actions that the 
+admin will perform and do not mention redirections.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddOffer_TC_V1.0_002</t>
+  </si>
+  <si>
+    <t>In Test case with id "TC_F_AddOffer_Admin_002",
+add restraunt name in test data.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddOffer_TC_V1.0_003</t>
+  </si>
+  <si>
+    <t>In any testcases that have blank test data, 
+remove the space from inside the double quotations to avoid confusion with spaces.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddOffer_TC_V1.0_004</t>
+  </si>
+  <si>
+    <t>Test case "TC_F_AddOffer_Admin_017" is duplicate.
+ It is the same as "F_AddOffer_Admin_003".
+Please remove it.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddRestraunt_TC_V1.0_001</t>
+  </si>
+  <si>
+    <t>Test case "TC_F_AddResturant_Admin_002" is duplicate. You are already verifying 
+that add button redirects you to AddMenuItem page in test case "TC_F_AddResturant_Admin_001"</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddRestraunt_TC_V1.0_002</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddRestraunt_TC_V1.0_003</t>
+  </si>
+  <si>
+    <t>In test case "TC_F_AddResturant_Admin_005",
+ Add the restraunt name in test data as blank.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddRestraunt_TC_V1.0_004</t>
+  </si>
+  <si>
+    <t>In test case "TC_F_AddResturant_Admin_006",
+ Add the restraunt logo in test data as blank.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddRestraunt_TC_V1.0_005</t>
+  </si>
+  <si>
+    <t>In test case "TC_F_AddResturant_Admin_007",
+ Add the restraunt name and restraunt logo in test data as blank.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddRestraunt_TC_V1.0_006</t>
+  </si>
+  <si>
+    <t>In test cases "TC_F_AddResturant_Admin_012" and "TC_F_AddResturant_Admin_013" the test description is incorrect. You should verify that those extentions are unacceptable.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddMenuItem_TC_V1.0_001</t>
+  </si>
+  <si>
+    <t>In the testcases steps, write only the actions that the admin will perform and do not mention redirections.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddMenuItem_TC_V1.0_002</t>
+  </si>
+  <si>
+    <t>In test case "TC_F_AddMenuItem_Admin_002", in the description, the 'ok' button is the one that redirects to the admin home page not 'add' button.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddMenuItem_TC_V1.0_003</t>
+  </si>
+  <si>
+    <t>In test case "TC_F_AddMenuItem_Admin_003", in the test steps, the user will have to login only.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddMenuItem_TC_V1.0_004</t>
+  </si>
+  <si>
+    <t>Use verify verb in test cases description instead of other verbs.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddMenuItem_TC_V1.0_005</t>
+  </si>
+  <si>
+    <t>In test case "TC_F_AddMenuItem_Admin_008", in test data add blank item name.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_Admin_AddMenuItem_TC_V1.0_006</t>
+  </si>
+  <si>
+    <t>Make the assumed expected results fields with the orange color.</t>
+  </si>
+  <si>
+    <t>F_REVIEW_User_HomePage_TC_V1.0_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case "TC_F_Home_User_002" is duplicate as you already verify
+the redirection to offers page in test case "TC_F_Home_User_001". </t>
+  </si>
+  <si>
+    <t>F_REVIEW_User_HomePage_TC_V1.0_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case "TC_F_Home_User_004" is duplicate as you already verify
+the redirection to the restraunt's menu page in test case "TC_F_Home_User_003". </t>
+  </si>
+  <si>
+    <t>F_REVIEW_User_OffersAndPromotions_TC_V1.0_001</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1027,6 +1155,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1138,7 +1272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1296,12 +1430,158 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="228">
+  <dxfs count="248">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -9032,44 +9312,44 @@
     <mergeCell ref="B16:J16"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F15 F18:F1048576">
-    <cfRule type="cellIs" dxfId="227" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="10" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="224" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="223" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="6" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="219" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9087,6 +9367,321 @@
       </x14:dataValidations>
     </ext>
   </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A3:N46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
+        <f>COUNTIFS(PMP_Review!F2:F1048576,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="4">
+        <f>COUNTIFS(SRS_Review!F2:F1048576,"Open")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="55"/>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <f>COUNTIFS(PMP_Review!F2:F1048576,"Closed")</f>
+        <v>14</v>
+      </c>
+      <c r="L4" s="56"/>
+      <c r="M4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="4">
+        <f>COUNTIFS(SRS_Review!F2:F1048576,"Closed")</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="55"/>
+      <c r="B5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="14">
+        <f>COUNTIFS(PMP_Review!F2:F1048576,"In Progress")</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="56"/>
+      <c r="M5" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" s="15">
+        <f>COUNTIFS(SRS_Review!F2:F1048576,"In Progress")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="55"/>
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="14">
+        <f>COUNTIFS(PMP_Review!F2:F1048576,"Need Approval")</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="56"/>
+      <c r="M6" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="15">
+        <f>COUNTIFS(SRS_Review!F2:F1048576,"Need Approval")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="55"/>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3">
+        <f>SUM(C3:C6)</f>
+        <v>14</v>
+      </c>
+      <c r="L7" s="56"/>
+      <c r="M7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="4">
+        <f>SUM(N3:N6)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="55" t="s">
+        <v>199</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="23">
+        <f>COUNTIF(WireFrame_Review!F2:F1048576,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="M23" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="N23" s="24">
+        <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"Open")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="55"/>
+      <c r="B24" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="23">
+        <f>COUNTIF(WireFrame_Review!F2:F1048576,"Closed")</f>
+        <v>19</v>
+      </c>
+      <c r="L24" s="56"/>
+      <c r="M24" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" s="24">
+        <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"Closed")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="55"/>
+      <c r="B25" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="23">
+        <f>COUNTIF(WireFrame_Review!F2:F1048576,"In Progress")</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="56"/>
+      <c r="M25" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="N25" s="24">
+        <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"In Progress")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="55"/>
+      <c r="B26" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="23">
+        <f>COUNTIF(WireFrame_Review!F2:F1048576,"Need Approval")</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="56"/>
+      <c r="M26" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="N26" s="24">
+        <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"Need Approval")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="55"/>
+      <c r="B27" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="23">
+        <f>SUM(C23:C26)</f>
+        <v>19</v>
+      </c>
+      <c r="L27" s="56"/>
+      <c r="M27" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="N27" s="24">
+        <f>SUM(N23:N26)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H34" s="25"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="23">
+        <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="L42" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="M42" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="N42" s="24">
+        <f>COUNTIF(Audit_Review!H2:H1048576,"Open")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="55"/>
+      <c r="B43" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="23">
+        <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Closed")</f>
+        <v>2</v>
+      </c>
+      <c r="L43" s="56"/>
+      <c r="M43" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="N43" s="24">
+        <f>COUNTIF(Audit_Review!H2:H1048576,"Closed")</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" s="55"/>
+      <c r="B44" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="23">
+        <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"In Progress")</f>
+        <v>0</v>
+      </c>
+      <c r="L44" s="56"/>
+      <c r="M44" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="N44" s="24">
+        <f>COUNTIF(Audit_Review!H2:H1048576,"In Progress")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" s="55"/>
+      <c r="B45" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="23">
+        <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Need Approval")</f>
+        <v>0</v>
+      </c>
+      <c r="L45" s="56"/>
+      <c r="M45" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="N45" s="24">
+        <f>COUNTIF(Audit_Review!H2:H1048576,"Need Approval")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="55"/>
+      <c r="B46" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="23">
+        <f>SUM(C42:C45)</f>
+        <v>2</v>
+      </c>
+      <c r="L46" s="56"/>
+      <c r="M46" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="N46" s="24">
+        <f>SUM(N42:N45)</f>
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="L3:L7"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="L23:L27"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="L42:L46"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9359,16 +9954,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="215" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9962,240 +10557,240 @@
     <mergeCell ref="A20:J20"/>
   </mergeCells>
   <conditionalFormatting sqref="F23:F1048576 F1:F3">
-    <cfRule type="cellIs" dxfId="211" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="77" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="78" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="79" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="80" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="207" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="73" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="74" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="75" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="76" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="203" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="69" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="70" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="71" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="72" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="199" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="65" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="66" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="67" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="68" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="195" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="61" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="62" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="63" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="64" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="191" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="57" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="58" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="59" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="60" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="187" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="53" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="54" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="55" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="56" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="183" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="49" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="50" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="51" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="52" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="179" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="45" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="46" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="47" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="48" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="175" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="41" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="42" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="43" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="44" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="171" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="37" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="38" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="39" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="40" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="167" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="21" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="22" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="23" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="163" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="17" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="18" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="19" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:F19">
-    <cfRule type="cellIs" dxfId="159" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="14" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="15" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21 H21">
-    <cfRule type="cellIs" dxfId="155" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="151" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="147" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10495,16 +11090,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="143" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11179,30 +11774,30 @@
     <mergeCell ref="B23:J23"/>
   </mergeCells>
   <conditionalFormatting sqref="F14:F21 F32:F38 F1:F12 F40:F1048576">
-    <cfRule type="cellIs" dxfId="139" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="135" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11396,16 +11991,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F14:F21 F23:F1048576 F1:F12">
-    <cfRule type="cellIs" dxfId="131" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11429,7 +12024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="G27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -12663,450 +13258,450 @@
     <mergeCell ref="A34:L34"/>
   </mergeCells>
   <conditionalFormatting sqref="H35:H1048576">
-    <cfRule type="cellIs" dxfId="127" priority="233" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="233" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="234" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="235" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="236" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="123" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="149" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="150" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="151" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="152" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="119" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="145" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="146" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="147" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="148" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H16">
-    <cfRule type="cellIs" dxfId="115" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="141" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="142" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="143" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="144" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H16">
-    <cfRule type="cellIs" dxfId="111" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="137" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="138" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="139" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="140" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="107" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="133" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="134" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="135" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="136" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="103" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="129" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="130" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="131" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="132" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="99" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="117" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="118" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="119" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="120" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="95" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="113" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="114" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="115" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="116" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="91" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="109" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="110" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="111" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="112" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="87" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="85" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="86" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="87" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="88" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="83" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="81" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="82" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="83" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="84" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="79" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="77" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="78" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="79" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="80" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="75" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="73" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="74" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="75" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="76" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="71" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="69" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="70" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="71" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="72" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="67" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="65" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="66" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="67" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="68" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="63" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="61" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="62" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="63" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="64" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="57" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="58" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="59" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="60" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="55" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="53" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="54" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="55" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="56" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="49" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="50" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="51" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="52" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:H31 H33">
-    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="45" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="46" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="47" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="48" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:H31 H33">
-    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="41" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="42" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="43" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="44" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="37" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="38" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="39" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="40" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="33" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="34" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="35" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="36" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H9">
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="29" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="30" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="31" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="32" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H9">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="25" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="26" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="27" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="28" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H6">
-    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="22" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="23" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H6">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="18" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="19" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="14" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13134,316 +13729,567 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A3:N46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC0C8B8-7956-4122-85A2-1A4F293B4470}">
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="46.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="59.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.21875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="1" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="F2" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
-        <f>COUNTIFS(PMP_Review!F2:F1048576,"Open")</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="4" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="F3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="4">
-        <f>COUNTIFS(SRS_Review!F2:F1048576,"Open")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3">
-        <f>COUNTIFS(PMP_Review!F2:F1048576,"Closed")</f>
-        <v>14</v>
-      </c>
-      <c r="L4" s="56"/>
-      <c r="M4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N4" s="4">
-        <f>COUNTIFS(SRS_Review!F2:F1048576,"Closed")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
-      <c r="B5" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="14">
-        <f>COUNTIFS(PMP_Review!F2:F1048576,"In Progress")</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="N5" s="15">
-        <f>COUNTIFS(SRS_Review!F2:F1048576,"In Progress")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="55"/>
-      <c r="B6" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="14">
-        <f>COUNTIFS(PMP_Review!F2:F1048576,"Need Approval")</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="56"/>
-      <c r="M6" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="N6" s="15">
-        <f>COUNTIFS(SRS_Review!F2:F1048576,"Need Approval")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3">
-        <f>SUM(C3:C6)</f>
-        <v>14</v>
-      </c>
-      <c r="L7" s="56"/>
-      <c r="M7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N7" s="4">
-        <f>SUM(N3:N6)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="55" t="s">
-        <v>199</v>
-      </c>
-      <c r="B23" s="23" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="F4" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="23">
-        <f>COUNTIF(WireFrame_Review!F2:F1048576,"Open")</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="M23" s="24" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="F5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="N23" s="24">
-        <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"Open")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="55"/>
-      <c r="B24" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="23">
-        <f>COUNTIF(WireFrame_Review!F2:F1048576,"Closed")</f>
-        <v>19</v>
-      </c>
-      <c r="L24" s="56"/>
-      <c r="M24" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="N24" s="24">
-        <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"Closed")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="55"/>
-      <c r="B25" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="23">
-        <f>COUNTIF(WireFrame_Review!F2:F1048576,"In Progress")</f>
-        <v>0</v>
-      </c>
-      <c r="L25" s="56"/>
-      <c r="M25" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="N25" s="24">
-        <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"In Progress")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="55"/>
-      <c r="B26" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="23">
-        <f>COUNTIF(WireFrame_Review!F2:F1048576,"Need Approval")</f>
-        <v>0</v>
-      </c>
-      <c r="L26" s="56"/>
-      <c r="M26" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="N26" s="24">
-        <f>COUNTIF(Risk_Managment_Plan_Review!F2:F1048576,"Need Approval")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="55"/>
-      <c r="B27" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="23">
-        <f>SUM(C23:C26)</f>
-        <v>19</v>
-      </c>
-      <c r="L27" s="56"/>
-      <c r="M27" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="N27" s="24">
-        <f>SUM(N23:N26)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="H34" s="25"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="55" t="s">
-        <v>111</v>
-      </c>
-      <c r="B42" s="23" t="s">
+    </row>
+    <row r="6" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="F7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="23">
-        <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Open")</f>
-        <v>0</v>
-      </c>
-      <c r="L42" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="M42" s="24" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="F8" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="N42" s="24">
-        <f>COUNTIF(Audit_Review!H2:H1048576,"Open")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" s="55"/>
-      <c r="B43" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="23">
-        <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Closed")</f>
-        <v>2</v>
-      </c>
-      <c r="L43" s="56"/>
-      <c r="M43" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="N43" s="24">
-        <f>COUNTIF(Audit_Review!H2:H1048576,"Closed")</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" s="55"/>
-      <c r="B44" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="23">
-        <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"In Progress")</f>
-        <v>0</v>
-      </c>
-      <c r="L44" s="56"/>
-      <c r="M44" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="N44" s="24">
-        <f>COUNTIF(Audit_Review!H2:H1048576,"In Progress")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" s="55"/>
-      <c r="B45" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C45" s="23">
-        <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Need Approval")</f>
-        <v>0</v>
-      </c>
-      <c r="L45" s="56"/>
-      <c r="M45" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="N45" s="24">
-        <f>COUNTIF(Audit_Review!H2:H1048576,"Need Approval")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" s="55"/>
-      <c r="B46" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="23">
-        <f>SUM(C42:C45)</f>
-        <v>2</v>
-      </c>
-      <c r="L46" s="56"/>
-      <c r="M46" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="N46" s="24">
-        <f>SUM(N42:N45)</f>
-        <v>36</v>
-      </c>
+    </row>
+    <row r="9" spans="1:10" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="F11" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="F12" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="F14" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="F15" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>306</v>
+      </c>
+      <c r="F16" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="F17" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="F18" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F19" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="F21" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="F22" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="F24" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="F25" s="58"/>
+    </row>
+    <row r="26" spans="1:10" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="F26" s="58"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="L3:L7"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="L23:L27"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="L42:L46"/>
-  </mergeCells>
+  <conditionalFormatting sqref="F1">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Review sheet with testCases review
</commit_message>
<xml_diff>
--- a/Monitor and Control/F_Review.xlsx
+++ b/Monitor and Control/F_Review.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2E159D18-4CAE-433C-B33C-39F62B59F17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08C787AD-37C4-43F9-BA46-9C66560AA454}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9745F89-9DF0-4011-8F5B-03B751CA6571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP_Review" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="SRS_Review" sheetId="3" r:id="rId6"/>
     <sheet name="Sequence_Diagrams_Review" sheetId="10" r:id="rId7"/>
     <sheet name="Audit_Review" sheetId="11" r:id="rId8"/>
-    <sheet name="TestCase_Part1_Review" sheetId="14" r:id="rId9"/>
+    <sheet name="TestCase_Review" sheetId="14" r:id="rId9"/>
     <sheet name="Progress_Chart" sheetId="4" r:id="rId10"/>
   </sheets>
   <externalReferences>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Audit_Review!$A$1:$L$1</definedName>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,9 +34,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -46,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="344">
   <si>
     <t>Raised By</t>
   </si>
@@ -1069,6 +1067,97 @@
   </si>
   <si>
     <t>F_REVIEW_User_OffersAndPromotions_TC_V1.0_001</t>
+  </si>
+  <si>
+    <t>F_Review_User_Confirm_Order_001</t>
+  </si>
+  <si>
+    <t>HagerHany</t>
+  </si>
+  <si>
+    <t>HagerNasser</t>
+  </si>
+  <si>
+    <t>Missed testcases to 
+check item price</t>
+  </si>
+  <si>
+    <t>F_Review_User_Confirm_Order_002</t>
+  </si>
+  <si>
+    <t>Missed testcases to 
+check Total price</t>
+  </si>
+  <si>
+    <t>F_Review_User_Confirm_Order_003</t>
+  </si>
+  <si>
+    <t>Missed testcases to 
+check discount</t>
+  </si>
+  <si>
+    <t>F_Review_User_Confirm_Order_004</t>
+  </si>
+  <si>
+    <t>Missed testcases to check offers link</t>
+  </si>
+  <si>
+    <t>F_Review_User_MenuItem_001</t>
+  </si>
+  <si>
+    <t>Some Test Cases has incorrect expected results
+TC_F_MenuItem_002
+TC_F_MenuItem_004</t>
+  </si>
+  <si>
+    <t>F_Review_User_MenuItem_002</t>
+  </si>
+  <si>
+    <t>Some Test Cases has no test
+data
+TC_F_MenuItem_001
+TC_F_MenuItem_004
+TC_F_MenuItem_005</t>
+  </si>
+  <si>
+    <t>F_Review_User_MenuItem_003</t>
+  </si>
+  <si>
+    <t>Missed testcases to check menuItem price</t>
+  </si>
+  <si>
+    <t>F_Review_AdminHome__001</t>
+  </si>
+  <si>
+    <t>preconditions are wrong need to be corrected
+TC_F_AdminHome_001</t>
+  </si>
+  <si>
+    <t>F_Review_AdminHome__002</t>
+  </si>
+  <si>
+    <t>Wrong expected results need to be corrected
+TC_F_AdminHome_002</t>
+  </si>
+  <si>
+    <t>F_Review_Registration__001</t>
+  </si>
+  <si>
+    <t>in TC_F_Reg_User_002 the expected Result is incorrect 
+Please Review The SRS</t>
+  </si>
+  <si>
+    <t>F_Review_Registration__002</t>
+  </si>
+  <si>
+    <t>missed test cases to validatethat fullnme can't contain special character</t>
+  </si>
+  <si>
+    <t>F_Review_Registration__003</t>
+  </si>
+  <si>
+    <t>in TC_F_Reg_User_005 the expected Result is incorrect 
+Please Review The SRS</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1404,6 +1493,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1430,10 +1528,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1441,7 +1536,35 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="248">
+  <dxfs count="252">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -9056,15 +9179,15 @@
     </row>
     <row r="8" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="50"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
@@ -9268,15 +9391,15 @@
     </row>
     <row r="16" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="50"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="53"/>
     </row>
     <row r="17" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
@@ -9312,44 +9435,44 @@
     <mergeCell ref="B16:J16"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F15 F18:F1048576">
-    <cfRule type="cellIs" dxfId="247" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="246" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="10" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="245" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="244" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="243" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="242" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="6" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="241" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="239" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="238" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="237" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="236" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9387,7 +9510,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="58" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -9397,7 +9520,7 @@
         <f>COUNTIFS(PMP_Review!F2:F1048576,"Open")</f>
         <v>0</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="59" t="s">
         <v>10</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -9409,7 +9532,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -9417,7 +9540,7 @@
         <f>COUNTIFS(PMP_Review!F2:F1048576,"Closed")</f>
         <v>14</v>
       </c>
-      <c r="L4" s="56"/>
+      <c r="L4" s="59"/>
       <c r="M4" s="4" t="s">
         <v>6</v>
       </c>
@@ -9427,7 +9550,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="14" t="s">
         <v>46</v>
       </c>
@@ -9435,7 +9558,7 @@
         <f>COUNTIFS(PMP_Review!F2:F1048576,"In Progress")</f>
         <v>0</v>
       </c>
-      <c r="L5" s="56"/>
+      <c r="L5" s="59"/>
       <c r="M5" s="15" t="s">
         <v>46</v>
       </c>
@@ -9445,7 +9568,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="55"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="14" t="s">
         <v>66</v>
       </c>
@@ -9453,7 +9576,7 @@
         <f>COUNTIFS(PMP_Review!F2:F1048576,"Need Approval")</f>
         <v>0</v>
       </c>
-      <c r="L6" s="56"/>
+      <c r="L6" s="59"/>
       <c r="M6" s="15" t="s">
         <v>66</v>
       </c>
@@ -9463,7 +9586,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -9471,7 +9594,7 @@
         <f>SUM(C3:C6)</f>
         <v>14</v>
       </c>
-      <c r="L7" s="56"/>
+      <c r="L7" s="59"/>
       <c r="M7" s="4" t="s">
         <v>9</v>
       </c>
@@ -9481,7 +9604,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="58" t="s">
         <v>199</v>
       </c>
       <c r="B23" s="23" t="s">
@@ -9491,7 +9614,7 @@
         <f>COUNTIF(WireFrame_Review!F2:F1048576,"Open")</f>
         <v>0</v>
       </c>
-      <c r="L23" s="56" t="s">
+      <c r="L23" s="59" t="s">
         <v>76</v>
       </c>
       <c r="M23" s="24" t="s">
@@ -9503,7 +9626,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="55"/>
+      <c r="A24" s="58"/>
       <c r="B24" s="23" t="s">
         <v>6</v>
       </c>
@@ -9511,7 +9634,7 @@
         <f>COUNTIF(WireFrame_Review!F2:F1048576,"Closed")</f>
         <v>19</v>
       </c>
-      <c r="L24" s="56"/>
+      <c r="L24" s="59"/>
       <c r="M24" s="24" t="s">
         <v>6</v>
       </c>
@@ -9521,7 +9644,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="55"/>
+      <c r="A25" s="58"/>
       <c r="B25" s="23" t="s">
         <v>46</v>
       </c>
@@ -9529,7 +9652,7 @@
         <f>COUNTIF(WireFrame_Review!F2:F1048576,"In Progress")</f>
         <v>0</v>
       </c>
-      <c r="L25" s="56"/>
+      <c r="L25" s="59"/>
       <c r="M25" s="24" t="s">
         <v>46</v>
       </c>
@@ -9539,7 +9662,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="55"/>
+      <c r="A26" s="58"/>
       <c r="B26" s="23" t="s">
         <v>66</v>
       </c>
@@ -9547,7 +9670,7 @@
         <f>COUNTIF(WireFrame_Review!F2:F1048576,"Need Approval")</f>
         <v>0</v>
       </c>
-      <c r="L26" s="56"/>
+      <c r="L26" s="59"/>
       <c r="M26" s="24" t="s">
         <v>66</v>
       </c>
@@ -9557,7 +9680,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="55"/>
+      <c r="A27" s="58"/>
       <c r="B27" s="23" t="s">
         <v>9</v>
       </c>
@@ -9565,7 +9688,7 @@
         <f>SUM(C23:C26)</f>
         <v>19</v>
       </c>
-      <c r="L27" s="56"/>
+      <c r="L27" s="59"/>
       <c r="M27" s="24" t="s">
         <v>9</v>
       </c>
@@ -9578,7 +9701,7 @@
       <c r="H34" s="25"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="55" t="s">
+      <c r="A42" s="58" t="s">
         <v>111</v>
       </c>
       <c r="B42" s="23" t="s">
@@ -9588,7 +9711,7 @@
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Open")</f>
         <v>0</v>
       </c>
-      <c r="L42" s="56" t="s">
+      <c r="L42" s="59" t="s">
         <v>129</v>
       </c>
       <c r="M42" s="24" t="s">
@@ -9600,7 +9723,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" s="55"/>
+      <c r="A43" s="58"/>
       <c r="B43" s="23" t="s">
         <v>6</v>
       </c>
@@ -9608,7 +9731,7 @@
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Closed")</f>
         <v>2</v>
       </c>
-      <c r="L43" s="56"/>
+      <c r="L43" s="59"/>
       <c r="M43" s="24" t="s">
         <v>6</v>
       </c>
@@ -9618,7 +9741,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" s="55"/>
+      <c r="A44" s="58"/>
       <c r="B44" s="23" t="s">
         <v>46</v>
       </c>
@@ -9626,7 +9749,7 @@
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"In Progress")</f>
         <v>0</v>
       </c>
-      <c r="L44" s="56"/>
+      <c r="L44" s="59"/>
       <c r="M44" s="24" t="s">
         <v>46</v>
       </c>
@@ -9636,7 +9759,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" s="55"/>
+      <c r="A45" s="58"/>
       <c r="B45" s="23" t="s">
         <v>66</v>
       </c>
@@ -9644,7 +9767,7 @@
         <f>COUNTIF(Sequence_Diagrams_Review!F2:F1048576,"Need Approval")</f>
         <v>0</v>
       </c>
-      <c r="L45" s="56"/>
+      <c r="L45" s="59"/>
       <c r="M45" s="24" t="s">
         <v>66</v>
       </c>
@@ -9654,7 +9777,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" s="55"/>
+      <c r="A46" s="58"/>
       <c r="B46" s="23" t="s">
         <v>9</v>
       </c>
@@ -9662,7 +9785,7 @@
         <f>SUM(C42:C45)</f>
         <v>2</v>
       </c>
-      <c r="L46" s="56"/>
+      <c r="L46" s="59"/>
       <c r="M46" s="24" t="s">
         <v>9</v>
       </c>
@@ -9954,16 +10077,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="235" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="234" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="232" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10352,16 +10475,16 @@
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="50"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
@@ -10494,16 +10617,16 @@
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="50"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
@@ -10557,240 +10680,240 @@
     <mergeCell ref="A20:J20"/>
   </mergeCells>
   <conditionalFormatting sqref="F23:F1048576 F1:F3">
-    <cfRule type="cellIs" dxfId="231" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="77" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="230" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="78" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="229" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="79" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="228" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="80" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="227" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="73" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="74" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="75" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="224" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="76" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="223" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="69" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="70" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="71" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="72" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="219" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="65" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="66" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="67" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="68" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="215" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="61" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="62" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="63" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="64" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="211" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="57" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="58" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="59" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="60" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="207" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="53" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="54" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="55" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="56" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="203" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="49" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="50" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="51" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="52" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="199" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="45" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="46" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="47" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="48" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="195" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="41" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="42" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="43" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="44" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="191" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="37" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="38" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="39" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="40" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="187" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="21" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="22" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="23" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="183" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="17" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="18" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="19" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:F19">
-    <cfRule type="cellIs" dxfId="179" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="14" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="15" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21 H21">
-    <cfRule type="cellIs" dxfId="175" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="171" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="167" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11090,16 +11213,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="163" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11487,15 +11610,15 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="50"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
@@ -11723,15 +11846,15 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="50"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="53"/>
     </row>
     <row r="24" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="45" t="s">
@@ -11774,30 +11897,30 @@
     <mergeCell ref="B23:J23"/>
   </mergeCells>
   <conditionalFormatting sqref="F14:F21 F32:F38 F1:F12 F40:F1048576">
-    <cfRule type="cellIs" dxfId="159" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="155" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11991,16 +12114,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F14:F21 F23:F1048576 F1:F12">
-    <cfRule type="cellIs" dxfId="151" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12025,7 +12148,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="K38" sqref="K38"/>
@@ -12330,18 +12453,18 @@
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="54"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="57"/>
     </row>
     <row r="11" spans="1:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -12940,18 +13063,18 @@
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="52"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="54"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="57"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
@@ -13114,18 +13237,18 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="52"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="54"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
+      <c r="L34" s="57"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="29" t="s">
@@ -13258,450 +13381,450 @@
     <mergeCell ref="A34:L34"/>
   </mergeCells>
   <conditionalFormatting sqref="H35:H1048576">
-    <cfRule type="cellIs" dxfId="147" priority="233" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="233" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="234" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="235" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="236" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="143" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="149" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="150" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="151" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="152" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="139" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="145" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="146" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="147" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="148" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H16">
-    <cfRule type="cellIs" dxfId="135" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="141" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="142" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="143" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="144" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H16">
-    <cfRule type="cellIs" dxfId="131" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="137" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="138" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="139" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="140" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="127" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="133" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="134" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="135" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="136" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H20">
-    <cfRule type="cellIs" dxfId="123" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="129" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="130" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="131" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="132" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="119" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="117" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="118" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="119" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="120" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="115" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="113" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="114" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="115" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="116" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="111" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="109" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="110" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="111" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="112" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="107" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="85" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="86" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="87" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="88" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="103" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="81" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="82" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="83" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="84" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="99" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="77" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="78" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="79" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="80" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="95" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="73" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="74" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="75" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="76" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="91" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="69" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="70" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="71" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="72" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="87" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="65" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="66" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="67" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="68" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="83" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="61" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="62" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="63" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="64" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="79" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="57" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="58" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="59" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="60" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="75" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="53" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="54" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="55" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="56" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="71" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="49" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="50" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="51" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="52" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:H31 H33">
-    <cfRule type="cellIs" dxfId="67" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="45" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="46" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="47" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="48" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:H31 H33">
-    <cfRule type="cellIs" dxfId="63" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="41" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="42" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="43" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="44" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="59" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="37" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="38" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="39" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="40" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="55" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="33" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="34" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="35" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="36" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H9">
-    <cfRule type="cellIs" dxfId="51" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="29" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="30" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="31" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="32" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H9">
-    <cfRule type="cellIs" dxfId="47" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="25" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="26" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="27" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="28" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H6">
-    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="21" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="22" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="23" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H6">
-    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="17" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="18" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="19" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="35" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="14" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="15" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13730,497 +13853,1240 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC0C8B8-7956-4122-85A2-1A4F293B4470}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:LE41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="59.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32" style="1" customWidth="1"/>
-    <col min="8" max="8" width="35.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="40.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="31.21875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="59.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32" style="1" customWidth="1"/>
+    <col min="9" max="9" width="35.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="40.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="31.21875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>172</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>280</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="G2" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>284</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="F3" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="G3" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>286</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="F4" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="G4" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>288</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="F5" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="F5" s="57" t="s">
+      <c r="G5" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>290</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="F7" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="G7" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>292</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="F8" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="G8" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>293</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="F9" s="20" t="s">
         <v>294</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="G9" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>295</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="F10" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="G10" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>297</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="F11" s="20" t="s">
         <v>298</v>
       </c>
-      <c r="F11" s="57" t="s">
+      <c r="G11" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>299</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="F12" s="20" t="s">
         <v>300</v>
       </c>
-      <c r="F12" s="57" t="s">
+      <c r="G12" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
-    </row>
-    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>301</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="F14" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="F14" s="57" t="s">
+      <c r="G14" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>303</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="F15" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="F15" s="57" t="s">
+      <c r="G15" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>305</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="F16" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="F16" s="57" t="s">
+      <c r="G16" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:317" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>307</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="F17" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="F17" s="57" t="s">
+      <c r="G17" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:317" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>309</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="F18" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="F18" s="57" t="s">
+      <c r="G18" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:317" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>311</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="G19" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:317" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:317" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>313</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="F21" s="20" t="s">
         <v>314</v>
       </c>
-      <c r="F21" s="57" t="s">
+      <c r="G21" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:317" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>315</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="F22" s="20" t="s">
         <v>316</v>
       </c>
-      <c r="F22" s="57" t="s">
+      <c r="G22" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:317" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="1:317" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>317</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="F24" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="F24" s="57" t="s">
+      <c r="G24" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="F25" s="58"/>
-    </row>
-    <row r="26" spans="1:10" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="F26" s="58"/>
-    </row>
+    <row r="25" spans="1:317" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:317" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E26" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I26" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="27" spans="1:317" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E27" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I27" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="28" spans="1:317" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E28" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I28" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="29" spans="1:317" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E29" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I29" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="30" spans="1:317" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="48"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="60"/>
+      <c r="S30" s="60"/>
+      <c r="T30" s="60"/>
+      <c r="U30" s="60"/>
+      <c r="V30" s="60"/>
+      <c r="W30" s="60"/>
+      <c r="X30" s="60"/>
+      <c r="Y30" s="60"/>
+      <c r="Z30" s="60"/>
+      <c r="AA30" s="60"/>
+      <c r="AB30" s="60"/>
+      <c r="AC30" s="60"/>
+      <c r="AD30" s="60"/>
+      <c r="AE30" s="60"/>
+      <c r="AF30" s="60"/>
+      <c r="AG30" s="60"/>
+      <c r="AH30" s="60"/>
+      <c r="AI30" s="60"/>
+      <c r="AJ30" s="60"/>
+      <c r="AK30" s="60"/>
+      <c r="AL30" s="60"/>
+      <c r="AM30" s="60"/>
+      <c r="AN30" s="60"/>
+      <c r="AO30" s="60"/>
+      <c r="AP30" s="60"/>
+      <c r="AQ30" s="60"/>
+      <c r="AR30" s="60"/>
+      <c r="AS30" s="60"/>
+      <c r="AT30" s="60"/>
+      <c r="AU30" s="60"/>
+      <c r="AV30" s="60"/>
+      <c r="AW30" s="60"/>
+      <c r="AX30" s="60"/>
+      <c r="AY30" s="60"/>
+      <c r="AZ30" s="60"/>
+      <c r="BA30" s="60"/>
+      <c r="BB30" s="60"/>
+      <c r="BC30" s="60"/>
+      <c r="BD30" s="60"/>
+      <c r="BE30" s="60"/>
+      <c r="BF30" s="60"/>
+      <c r="BG30" s="60"/>
+      <c r="BH30" s="60"/>
+      <c r="BI30" s="60"/>
+      <c r="BJ30" s="60"/>
+      <c r="BK30" s="60"/>
+      <c r="BL30" s="60"/>
+      <c r="BM30" s="60"/>
+      <c r="BN30" s="60"/>
+      <c r="BO30" s="60"/>
+      <c r="BP30" s="60"/>
+      <c r="BQ30" s="60"/>
+      <c r="BR30" s="60"/>
+      <c r="BS30" s="60"/>
+      <c r="BT30" s="60"/>
+      <c r="BU30" s="60"/>
+      <c r="BV30" s="60"/>
+      <c r="BW30" s="60"/>
+      <c r="BX30" s="60"/>
+      <c r="BY30" s="60"/>
+      <c r="BZ30" s="60"/>
+      <c r="CA30" s="60"/>
+      <c r="CB30" s="60"/>
+      <c r="CC30" s="60"/>
+      <c r="CD30" s="60"/>
+      <c r="CE30" s="60"/>
+      <c r="CF30" s="60"/>
+      <c r="CG30" s="60"/>
+      <c r="CH30" s="60"/>
+      <c r="CI30" s="60"/>
+      <c r="CJ30" s="60"/>
+      <c r="CK30" s="60"/>
+      <c r="CL30" s="60"/>
+      <c r="CM30" s="60"/>
+      <c r="CN30" s="60"/>
+      <c r="CO30" s="60"/>
+      <c r="CP30" s="60"/>
+      <c r="CQ30" s="60"/>
+      <c r="CR30" s="60"/>
+      <c r="CS30" s="60"/>
+      <c r="CT30" s="60"/>
+      <c r="CU30" s="60"/>
+      <c r="CV30" s="60"/>
+      <c r="CW30" s="60"/>
+      <c r="CX30" s="60"/>
+      <c r="CY30" s="60"/>
+      <c r="CZ30" s="60"/>
+      <c r="DA30" s="60"/>
+      <c r="DB30" s="60"/>
+      <c r="DC30" s="60"/>
+      <c r="DD30" s="60"/>
+      <c r="DE30" s="60"/>
+      <c r="DF30" s="60"/>
+      <c r="DG30" s="60"/>
+      <c r="DH30" s="60"/>
+      <c r="DI30" s="60"/>
+      <c r="DJ30" s="60"/>
+      <c r="DK30" s="60"/>
+      <c r="DL30" s="60"/>
+      <c r="DM30" s="60"/>
+      <c r="DN30" s="60"/>
+      <c r="DO30" s="60"/>
+      <c r="DP30" s="60"/>
+      <c r="DQ30" s="60"/>
+      <c r="DR30" s="60"/>
+      <c r="DS30" s="60"/>
+      <c r="DT30" s="60"/>
+      <c r="DU30" s="60"/>
+      <c r="DV30" s="60"/>
+      <c r="DW30" s="60"/>
+      <c r="DX30" s="60"/>
+      <c r="DY30" s="60"/>
+      <c r="DZ30" s="60"/>
+      <c r="EA30" s="60"/>
+      <c r="EB30" s="60"/>
+      <c r="EC30" s="60"/>
+      <c r="ED30" s="60"/>
+      <c r="EE30" s="60"/>
+      <c r="EF30" s="60"/>
+      <c r="EG30" s="60"/>
+      <c r="EH30" s="60"/>
+      <c r="EI30" s="60"/>
+      <c r="EJ30" s="60"/>
+      <c r="EK30" s="60"/>
+      <c r="EL30" s="60"/>
+      <c r="EM30" s="60"/>
+      <c r="EN30" s="60"/>
+      <c r="EO30" s="60"/>
+      <c r="EP30" s="60"/>
+      <c r="EQ30" s="60"/>
+      <c r="ER30" s="60"/>
+      <c r="ES30" s="60"/>
+      <c r="ET30" s="60"/>
+      <c r="EU30" s="60"/>
+      <c r="EV30" s="60"/>
+      <c r="EW30" s="60"/>
+      <c r="EX30" s="60"/>
+      <c r="EY30" s="60"/>
+      <c r="EZ30" s="60"/>
+      <c r="FA30" s="60"/>
+      <c r="FB30" s="60"/>
+      <c r="FC30" s="60"/>
+      <c r="FD30" s="60"/>
+      <c r="FE30" s="60"/>
+      <c r="FF30" s="60"/>
+      <c r="FG30" s="60"/>
+      <c r="FH30" s="60"/>
+      <c r="FI30" s="60"/>
+      <c r="FJ30" s="60"/>
+      <c r="FK30" s="60"/>
+      <c r="FL30" s="60"/>
+      <c r="FM30" s="60"/>
+      <c r="FN30" s="60"/>
+      <c r="FO30" s="60"/>
+      <c r="FP30" s="60"/>
+      <c r="FQ30" s="60"/>
+      <c r="FR30" s="60"/>
+      <c r="FS30" s="60"/>
+      <c r="FT30" s="60"/>
+      <c r="FU30" s="60"/>
+      <c r="FV30" s="60"/>
+      <c r="FW30" s="60"/>
+      <c r="FX30" s="60"/>
+      <c r="FY30" s="60"/>
+      <c r="FZ30" s="60"/>
+      <c r="GA30" s="60"/>
+      <c r="GB30" s="60"/>
+      <c r="GC30" s="60"/>
+      <c r="GD30" s="60"/>
+      <c r="GE30" s="60"/>
+      <c r="GF30" s="60"/>
+      <c r="GG30" s="60"/>
+      <c r="GH30" s="60"/>
+      <c r="GI30" s="60"/>
+      <c r="GJ30" s="60"/>
+      <c r="GK30" s="60"/>
+      <c r="GL30" s="60"/>
+      <c r="GM30" s="60"/>
+      <c r="GN30" s="60"/>
+      <c r="GO30" s="60"/>
+      <c r="GP30" s="60"/>
+      <c r="GQ30" s="60"/>
+      <c r="GR30" s="60"/>
+      <c r="GS30" s="60"/>
+      <c r="GT30" s="60"/>
+      <c r="GU30" s="60"/>
+      <c r="GV30" s="60"/>
+      <c r="GW30" s="60"/>
+      <c r="GX30" s="60"/>
+      <c r="GY30" s="60"/>
+      <c r="GZ30" s="60"/>
+      <c r="HA30" s="60"/>
+      <c r="HB30" s="60"/>
+      <c r="HC30" s="60"/>
+      <c r="HD30" s="60"/>
+      <c r="HE30" s="60"/>
+      <c r="HF30" s="60"/>
+      <c r="HG30" s="60"/>
+      <c r="HH30" s="60"/>
+      <c r="HI30" s="60"/>
+      <c r="HJ30" s="60"/>
+      <c r="HK30" s="60"/>
+      <c r="HL30" s="60"/>
+      <c r="HM30" s="60"/>
+      <c r="HN30" s="60"/>
+      <c r="HO30" s="60"/>
+      <c r="HP30" s="60"/>
+      <c r="HQ30" s="60"/>
+      <c r="HR30" s="60"/>
+      <c r="HS30" s="60"/>
+      <c r="HT30" s="60"/>
+      <c r="HU30" s="60"/>
+      <c r="HV30" s="60"/>
+      <c r="HW30" s="60"/>
+      <c r="HX30" s="60"/>
+      <c r="HY30" s="60"/>
+      <c r="HZ30" s="60"/>
+      <c r="IA30" s="60"/>
+      <c r="IB30" s="60"/>
+      <c r="IC30" s="60"/>
+      <c r="ID30" s="60"/>
+      <c r="IE30" s="60"/>
+      <c r="IF30" s="60"/>
+      <c r="IG30" s="60"/>
+      <c r="IH30" s="60"/>
+      <c r="II30" s="60"/>
+      <c r="IJ30" s="60"/>
+      <c r="IK30" s="60"/>
+      <c r="IL30" s="60"/>
+      <c r="IM30" s="60"/>
+      <c r="IN30" s="60"/>
+      <c r="IO30" s="60"/>
+      <c r="IP30" s="60"/>
+      <c r="IQ30" s="60"/>
+      <c r="IR30" s="60"/>
+      <c r="IS30" s="60"/>
+      <c r="IT30" s="60"/>
+      <c r="IU30" s="60"/>
+      <c r="IV30" s="60"/>
+      <c r="IW30" s="60"/>
+      <c r="IX30" s="60"/>
+      <c r="IY30" s="60"/>
+      <c r="IZ30" s="60"/>
+      <c r="JA30" s="60"/>
+      <c r="JB30" s="60"/>
+      <c r="JC30" s="60"/>
+      <c r="JD30" s="60"/>
+      <c r="JE30" s="60"/>
+      <c r="JF30" s="60"/>
+      <c r="JG30" s="60"/>
+      <c r="JH30" s="60"/>
+      <c r="JI30" s="60"/>
+      <c r="JJ30" s="60"/>
+      <c r="JK30" s="60"/>
+      <c r="JL30" s="60"/>
+      <c r="JM30" s="60"/>
+      <c r="JN30" s="60"/>
+      <c r="JO30" s="60"/>
+      <c r="JP30" s="60"/>
+      <c r="JQ30" s="60"/>
+      <c r="JR30" s="60"/>
+      <c r="JS30" s="60"/>
+      <c r="JT30" s="60"/>
+      <c r="JU30" s="60"/>
+      <c r="JV30" s="60"/>
+      <c r="JW30" s="60"/>
+      <c r="JX30" s="60"/>
+      <c r="JY30" s="60"/>
+      <c r="JZ30" s="60"/>
+      <c r="KA30" s="60"/>
+      <c r="KB30" s="60"/>
+      <c r="KC30" s="60"/>
+      <c r="KD30" s="60"/>
+      <c r="KE30" s="60"/>
+      <c r="KF30" s="60"/>
+      <c r="KG30" s="60"/>
+      <c r="KH30" s="60"/>
+      <c r="KI30" s="60"/>
+      <c r="KJ30" s="60"/>
+      <c r="KK30" s="60"/>
+      <c r="KL30" s="60"/>
+      <c r="KM30" s="60"/>
+      <c r="KN30" s="60"/>
+      <c r="KO30" s="60"/>
+      <c r="KP30" s="60"/>
+      <c r="KQ30" s="60"/>
+      <c r="KR30" s="60"/>
+      <c r="KS30" s="60"/>
+      <c r="KT30" s="60"/>
+      <c r="KU30" s="60"/>
+      <c r="KV30" s="60"/>
+      <c r="KW30" s="60"/>
+      <c r="KX30" s="60"/>
+      <c r="KY30" s="60"/>
+      <c r="KZ30" s="60"/>
+      <c r="LA30" s="60"/>
+      <c r="LB30" s="60"/>
+      <c r="LC30" s="60"/>
+      <c r="LD30" s="60"/>
+      <c r="LE30" s="49"/>
+    </row>
+    <row r="31" spans="1:317" customFormat="1" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E31" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I31" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="32" spans="1:317" customFormat="1" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E32" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I32" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E33" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I33" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:9" customFormat="1" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E35" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I35" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E36" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I36" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:9" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E38" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I38" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E39" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I39" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E40" s="47">
+        <v>44707</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I40" s="47">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="F1">
+  <conditionalFormatting sqref="G1">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
     <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -14234,7 +15100,7 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
+  <conditionalFormatting sqref="G13">
     <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -14248,7 +15114,7 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
+  <conditionalFormatting sqref="G20">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -14262,7 +15128,7 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20">
+  <conditionalFormatting sqref="G23">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
@@ -14276,7 +15142,7 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23">
+  <conditionalFormatting sqref="G25">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>

</xml_diff>